<commit_message>
fix duplicates in properties
</commit_message>
<xml_diff>
--- a/datageneration/data/Spot_primary_keys_bundles.xlsx
+++ b/datageneration/data/Spot_primary_keys_bundles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28103"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschewelle.sharepoint.com/teams/GR-GR-ReCo-KID2/Freigegebene Dokumente/General/03_Ongoing Work/03C_MS_Spot - ongoing/03Cc_Development/Key-Value Pairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D9BDCA3-1D57-4AB3-BFEB-5B5BE0811672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3704B6C-DDD3-4CC0-880F-C37AA5928B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24000" yWindow="500" windowWidth="25720" windowHeight="26260" xr2:uid="{0ED01DE8-A235-1045-8C96-52557544134F}"/>
+    <workbookView xWindow="14420" yWindow="500" windowWidth="35300" windowHeight="26260" xr2:uid="{0ED01DE8-A235-1045-8C96-52557544134F}"/>
   </bookViews>
   <sheets>
     <sheet name="Bundles - cleaned up props" sheetId="1" r:id="rId1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4251" uniqueCount="1311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4254" uniqueCount="1314">
   <si>
     <t>index</t>
   </si>
@@ -2179,1708 +2179,1717 @@
     <t>power=terminal</t>
   </si>
   <si>
+    <t>power tower|power pole|electricity tower</t>
+  </si>
+  <si>
+    <t>power=tower, power=pole</t>
+  </si>
+  <si>
+    <t>abandoned|disused railway track|decommissioned railroad|Abandoned train track|disused railway|extinct line|deserted train track</t>
+  </si>
+  <si>
+    <t>railway=abandoned, railway=disused</t>
+  </si>
+  <si>
+    <t>railway under construction|railway repair</t>
+  </si>
+  <si>
+    <t>railway=construction</t>
+  </si>
+  <si>
+    <t>railroad track|Railway track|train track|train line</t>
+  </si>
+  <si>
+    <t>railway=rail, railway=light_rail, railway=miniature, railway=narrow_gauge, railway=subway, railway=tram, railway=route</t>
+  </si>
+  <si>
+    <t>high-speed train track|high speed train track</t>
+  </si>
+  <si>
+    <t>railway=rail AND highspeed=yes</t>
+  </si>
+  <si>
+    <t>tram track|tram|subway|light rail|subway track|metro|underground|tube|rapid transit</t>
+  </si>
+  <si>
+    <t>railway=subway, railway=tram, railway=light_rail</t>
+  </si>
+  <si>
+    <t>railway bridge|railroad viaduct|train bridge|railroad bridge|trestle bridge</t>
+  </si>
+  <si>
+    <t>railway=***any*** AND bridge=yes</t>
+  </si>
+  <si>
+    <t>railway cutting|submerged railway|sunken railway|under-level railway</t>
+  </si>
+  <si>
+    <t>cutting=yes</t>
+  </si>
+  <si>
+    <t>railway tunnel|train tunnel|metro tunnel|railway underpass|subway tunnel|railroad tunnel</t>
+  </si>
+  <si>
+    <t>railway=***any*** AND tunnel=yes</t>
+  </si>
+  <si>
+    <t>railway crossing|level crossing|grade crossing|pedestrian railway crossing</t>
+  </si>
+  <si>
+    <t>railway=crossing, railway=level_crossing, railway=tram_level_crossing, railway=railway_crossing</t>
+  </si>
+  <si>
+    <t>railway signal|railroad signal|railway light|train signal|trackside signal|railroad light|train signaling lights</t>
+  </si>
+  <si>
+    <t>railway=signal</t>
+  </si>
+  <si>
+    <t>railway switch|track switch|railroad switch|train switch|train crossover</t>
+  </si>
+  <si>
+    <t>railway=switch</t>
+  </si>
+  <si>
+    <t>turntable|rotating train platform|revolving train platform</t>
+  </si>
+  <si>
+    <t>railway=turntable</t>
+  </si>
+  <si>
+    <t>alcohol shop</t>
+  </si>
+  <si>
+    <t>shop=alcohol</t>
+  </si>
+  <si>
+    <t>bakery</t>
+  </si>
+  <si>
+    <t>shop=bakery</t>
+  </si>
+  <si>
+    <t>department store|large store</t>
+  </si>
+  <si>
+    <t>shop=department_store</t>
+  </si>
+  <si>
+    <t>mall|shopping centre</t>
+  </si>
+  <si>
+    <t>shop=mall</t>
+  </si>
+  <si>
+    <t>supermarket|discount|wholesale|discounter</t>
+  </si>
+  <si>
+    <t>shop=supermarket, building=supermarket, shop=discounter, shop=wholesale</t>
+  </si>
+  <si>
+    <t>clothes shop|clothing store|fashion store|boutique|fashion accessories</t>
+  </si>
+  <si>
+    <t>shop=clothes, shop=fashion, shop=boutique, shop=fashion_accessories</t>
+  </si>
+  <si>
+    <t>fabric shop</t>
+  </si>
+  <si>
+    <t>shop=fabric</t>
+  </si>
+  <si>
+    <t>jewelry shop</t>
+  </si>
+  <si>
+    <t>shop=jewelry</t>
+  </si>
+  <si>
+    <t>shoe shop</t>
+  </si>
+  <si>
+    <t>shop=shoes</t>
+  </si>
+  <si>
+    <t>charity shop</t>
+  </si>
+  <si>
+    <t>shop=charity</t>
+  </si>
+  <si>
+    <t>second hand shop</t>
+  </si>
+  <si>
+    <t>shop=second_hand</t>
+  </si>
+  <si>
+    <t>beauty shop|nail salon</t>
+  </si>
+  <si>
+    <t>shop=beauty</t>
+  </si>
+  <si>
+    <t>hairdresser</t>
+  </si>
+  <si>
+    <t>shop=hairdresser</t>
+  </si>
+  <si>
+    <t>medical supply store</t>
+  </si>
+  <si>
+    <t>shop=medical_supply</t>
+  </si>
+  <si>
+    <t>tattoo shop|tattoo parlour</t>
+  </si>
+  <si>
+    <t>shop=tattoo</t>
+  </si>
+  <si>
+    <t>doityourself shop|DIY shop</t>
+  </si>
+  <si>
+    <t>shop=doityourself</t>
+  </si>
+  <si>
+    <t>florist</t>
+  </si>
+  <si>
+    <t>shop=florist</t>
+  </si>
+  <si>
+    <t>electronics shop</t>
+  </si>
+  <si>
+    <t>shop=electronics</t>
+  </si>
+  <si>
+    <t>mobile phone shop</t>
+  </si>
+  <si>
+    <t>shop=mobile_phone</t>
+  </si>
+  <si>
+    <t>bicycle shop</t>
+  </si>
+  <si>
+    <t>shop=bicycle</t>
+  </si>
+  <si>
+    <t>boat shop</t>
+  </si>
+  <si>
+    <t>shop=boat</t>
+  </si>
+  <si>
+    <t>car shop|car repair shop|car repair</t>
+  </si>
+  <si>
+    <t>shop=car, shop=car_repair, shop=car_parts</t>
+  </si>
+  <si>
+    <t>fuel shop</t>
+  </si>
+  <si>
+    <t>shop=fuel</t>
+  </si>
+  <si>
+    <t>hunting shop</t>
+  </si>
+  <si>
+    <t>shop=hunting</t>
+  </si>
+  <si>
+    <t>military surplus shop</t>
+  </si>
+  <si>
+    <t>shop=military_surplus</t>
+  </si>
+  <si>
+    <t>motorcycle shop|motorcycle rental</t>
+  </si>
+  <si>
+    <t>shop=motorcycle, amenity=motorcycle_rental</t>
+  </si>
+  <si>
+    <t>sports shop| sport shop</t>
+  </si>
+  <si>
+    <t>shop=sports</t>
+  </si>
+  <si>
+    <t>art store|art shop</t>
+  </si>
+  <si>
+    <t>shop=art</t>
+  </si>
+  <si>
+    <t>Antique Shop|antiques shop|vintage store|antiques store|antiquities shop</t>
+  </si>
+  <si>
+    <t>shop=antiques</t>
+  </si>
+  <si>
+    <t>camera shop</t>
+  </si>
+  <si>
+    <t>shop=camera</t>
+  </si>
+  <si>
+    <t>music shop | instrument shop</t>
+  </si>
+  <si>
+    <t>shop=music, shop=musical_instrument</t>
+  </si>
+  <si>
+    <t>book shop|book store</t>
+  </si>
+  <si>
+    <t>shop=books</t>
+  </si>
+  <si>
+    <t>lottery shop</t>
+  </si>
+  <si>
+    <t>shop=lottery</t>
+  </si>
+  <si>
+    <t>laundry shop|laundry place|self service laundry</t>
+  </si>
+  <si>
+    <t>shop=laundry</t>
+  </si>
+  <si>
+    <t>travel agency</t>
+  </si>
+  <si>
+    <t>shop=travel_agency</t>
+  </si>
+  <si>
+    <t>weapon shop</t>
+  </si>
+  <si>
+    <t>shop=weapons</t>
+  </si>
+  <si>
+    <t>vacant shop</t>
+  </si>
+  <si>
+    <t>shop=vacant</t>
+  </si>
+  <si>
+    <t>baseball facility|baseball field</t>
+  </si>
+  <si>
+    <t>sport=baseball</t>
+  </si>
+  <si>
+    <t>basketball facility|basketball field</t>
+  </si>
+  <si>
+    <t>sport=basketball</t>
+  </si>
+  <si>
+    <t>golf facility|golf course</t>
+  </si>
+  <si>
+    <t>sport=golf, golf=***any***, leisure=golf_course</t>
+  </si>
+  <si>
+    <t>mini golf|miniature golf|putt-putt|crazy golf</t>
+  </si>
+  <si>
+    <t>leisure=miniature_golf</t>
+  </si>
+  <si>
+    <t>disc golf|disc golf course</t>
+  </si>
+  <si>
+    <t>disc_golf=***any***, leisure=disc_golf_course</t>
+  </si>
+  <si>
+    <t>Bowling Alley|bowling center</t>
+  </si>
+  <si>
+    <t>leisure=bowling_alley</t>
+  </si>
+  <si>
+    <t>ice skating field|ice skating hall|ice hockey</t>
+  </si>
+  <si>
+    <t>sport=ice_skating, sport=ice_hockey</t>
+  </si>
+  <si>
+    <t>sports facility|sports hall|sports center|sports club|athletics club|sporting club|sports association|sports society</t>
+  </si>
+  <si>
+    <t>sport=multi, building=sports_hall, club=sport, leisure=sports_hall</t>
+  </si>
+  <si>
+    <t>soccer field| soccer hall|soccer facility</t>
+  </si>
+  <si>
+    <t>sport=soccer</t>
+  </si>
+  <si>
+    <t>tennis court|tennis facility</t>
+  </si>
+  <si>
+    <t>sport=tennis</t>
+  </si>
+  <si>
+    <t>data center</t>
+  </si>
+  <si>
+    <t>telecom=data_center</t>
+  </si>
+  <si>
+    <t>alpine hut</t>
+  </si>
+  <si>
+    <t>tourism=alpine_hut</t>
+  </si>
+  <si>
+    <t>aquarium</t>
+  </si>
+  <si>
+    <t>tourism=aquarium</t>
+  </si>
+  <si>
+    <t>tourist attraction</t>
+  </si>
+  <si>
+    <t>tourism=attraction</t>
+  </si>
+  <si>
+    <t>parking lot for campers|caravan site|parking area for motorhomes</t>
+  </si>
+  <si>
+    <t>tourism=caravan_site</t>
+  </si>
+  <si>
+    <t>chalet</t>
+  </si>
+  <si>
+    <t>tourism=chalet</t>
+  </si>
+  <si>
+    <t>guest house</t>
+  </si>
+  <si>
+    <t>tourism=guest_house</t>
+  </si>
+  <si>
+    <t>hostel</t>
+  </si>
+  <si>
+    <t>tourism=hostel</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>tourism=hotel, building=hotel</t>
+  </si>
+  <si>
+    <t>tourist information</t>
+  </si>
+  <si>
+    <t>tourism=information</t>
+  </si>
+  <si>
+    <t>motel</t>
+  </si>
+  <si>
+    <t>tourism=motel, building=motel</t>
+  </si>
+  <si>
+    <t>museum</t>
+  </si>
+  <si>
+    <t>tourism=museum, building=museum</t>
+  </si>
+  <si>
+    <t>picnic site|picnic table|picnic shelter|picnic pavilion</t>
+  </si>
+  <si>
+    <t>tourism=picnic_site, leisure=picnic_table, amenity=shelter AND shelter_type=picnic_shelter</t>
+  </si>
+  <si>
+    <t>amusement park|carnival|fairground|funfair|festival ground|Fair|theme park</t>
+  </si>
+  <si>
+    <t>tourism=theme_park, landuse=fairground, landuse=recreation_ground, recreation_ground=showground, amenity=festival_grounds, leisure=festival_grounds, attraction=big_wheel AND attraction=roller_coaster</t>
+  </si>
+  <si>
+    <t>viewpoint|view point</t>
+  </si>
+  <si>
+    <t>tourism=viewpoint</t>
+  </si>
+  <si>
+    <t>zoo</t>
+  </si>
+  <si>
+    <t>tourism=zoo</t>
+  </si>
+  <si>
+    <t>canal|stream|river|channelstream area|creek|brook|watercourse|surge</t>
+  </si>
+  <si>
+    <t>water=river, water=stream, water=canal, waterway=river, waterway=stream, waterway=canal, water=oxbow</t>
+  </si>
+  <si>
+    <t>ditch</t>
+  </si>
+  <si>
+    <t>water=ditch, waterway=drain, waterway=ditch, barrier=ditch</t>
+  </si>
+  <si>
+    <t>lock for boats|lock</t>
+  </si>
+  <si>
+    <t>water=lock</t>
+  </si>
+  <si>
+    <t>lake|pond</t>
+  </si>
+  <si>
+    <t>water=lake, water=pond, landuse=pond</t>
+  </si>
+  <si>
+    <t>basin|reservoir|salt pond|water reservoir|wastewater basin</t>
+  </si>
+  <si>
+    <t>water=basin, landuse=basin, landuse=reservoir, landuse=salt_pond, water=basin, water=reservoir, man_made=reservoir_covered, water=wastewater</t>
+  </si>
+  <si>
+    <t>lagoon</t>
+  </si>
+  <si>
+    <t>water=lagoon</t>
+  </si>
+  <si>
+    <t>moat</t>
+  </si>
+  <si>
+    <t>water=moat</t>
+  </si>
+  <si>
+    <t>wastewater</t>
+  </si>
+  <si>
+    <t>water=wastewater</t>
+  </si>
+  <si>
+    <t>ship repair dock|dry dock|boatyard|boat storage</t>
+  </si>
+  <si>
+    <t>waterway=dock, waterway=boatyard, amenity=boat_storage</t>
+  </si>
+  <si>
+    <t>dam</t>
+  </si>
+  <si>
+    <t>waterway=dam</t>
+  </si>
+  <si>
+    <t>weir</t>
+  </si>
+  <si>
+    <t>waterway=weir</t>
+  </si>
+  <si>
+    <t>waterfall</t>
+  </si>
+  <si>
+    <t>waterway=waterfall</t>
+  </si>
+  <si>
+    <t>boat fuelling station|ship fuelling station</t>
+  </si>
+  <si>
+    <t>waterway=fuel</t>
+  </si>
+  <si>
+    <t>street name</t>
+  </si>
+  <si>
+    <t>addr:street~***any***</t>
+  </si>
+  <si>
+    <t>name|brand|brand name</t>
+  </si>
+  <si>
+    <t>name~***example***, brand~***example***</t>
+  </si>
+  <si>
+    <t>toll road</t>
+  </si>
+  <si>
+    <t>toll=yes</t>
+  </si>
+  <si>
+    <t>city limit sign</t>
+  </si>
+  <si>
+    <t>traffic_sign=city_limit</t>
+  </si>
+  <si>
+    <t>living street|neighbourhood street|residential road</t>
+  </si>
+  <si>
+    <t>highway=residential, highway=living_street, highway=service</t>
+  </si>
+  <si>
+    <t>divided highway|dual carriageway road|Dual carriageway</t>
+  </si>
+  <si>
+    <t>dual_carriageway=yes, area:highway=traffic_island</t>
+  </si>
+  <si>
+    <t>slip course|slip track|slip training</t>
+  </si>
+  <si>
+    <t>leisure=slipway</t>
+  </si>
+  <si>
+    <t>monorail|single rail system|monorail track</t>
+  </si>
+  <si>
+    <t>railway=monorail</t>
+  </si>
+  <si>
+    <t>funicular|cable railway|incline railway</t>
+  </si>
+  <si>
+    <t>railway=funicular</t>
+  </si>
+  <si>
+    <t>Train yard|railyard|rail yard|train depot</t>
+  </si>
+  <si>
+    <t>landuse=depot, service=yard, landuse=railway</t>
+  </si>
+  <si>
+    <t>inlet|Estuary|baymouth bar</t>
+  </si>
+  <si>
+    <t>estuary=yes</t>
+  </si>
+  <si>
+    <t>skyscraper|condominium|tall building|high-rise apartment|high-rise building|skyline</t>
+  </si>
+  <si>
+    <t>building=***any*** AND building:levels&gt;10</t>
+  </si>
+  <si>
+    <t>clear cut patch|logging|clear cut area|Logging area|deforested area|strip clearcut</t>
+  </si>
+  <si>
+    <t>landuse=logging, man_made=clearcut, man_made=cutline</t>
+  </si>
+  <si>
+    <t>street lane|Car lane|traffic lane</t>
+  </si>
+  <si>
+    <t>lanes=***numeric***</t>
+  </si>
+  <si>
+    <t>carpool lane|HOV lane|High-occupancy vehicle lane</t>
+  </si>
+  <si>
+    <t>["hov:lanes:forward:conditional"|"hov:lanes:backward:conditional"|"hov:lanes:forward"|"hov:lanes:backward"|"hov:lanes:conditional"|"hov:lanes"]=designated</t>
+  </si>
+  <si>
+    <t>lanes in each direction|lanes going in each direction</t>
+  </si>
+  <si>
+    <t>lanes:forward=***numeric*** AND lanes:backward=***numeric***</t>
+  </si>
+  <si>
+    <t>train station|station|railway station|railway passenger station|railroad station|train platform|train stopping location</t>
+  </si>
+  <si>
+    <t>railway=station, public_transport=station AND train=yes,public_transport=platform AND train=yes, public_transport=stop_position AND train=yes, railway=halt, railway=platform, building=train_station</t>
+  </si>
+  <si>
+    <t>bus stop|bus platform|Bus bay|coach stop area|trolleybus station|trolleybus terminal|trolleybus stopping location</t>
+  </si>
+  <si>
+    <t>highway=bus_stop, bus_bay=both, bus_bay=left, bus_bay=right, public_transport=stop_position AND bus=yes, public_transport=stop_area, public_transport=station AND trolleybus=yes, public_transport=platform AND trolleybus=yes, public_transport=platform AND trolleybus=yes, public_transport=platform AND bus=yes, public_transport=stop_position AND trolleybus=yes, public_transport=platform AND trolleybus=yes</t>
+  </si>
+  <si>
+    <t>bus station|public bus transport station|bus transit station|bus commuter station|bus transport hub|bus interchangeterminus|coach station|</t>
+  </si>
+  <si>
+    <t>public_transport=platform AND bus=yes, public_transport=station AND bus=yes, amenity=bus_station, highway=platform AND bus=yes</t>
+  </si>
+  <si>
+    <t>Tram Stop|Tram Stopping location|Tram Station|Tram Platform</t>
+  </si>
+  <si>
+    <t>public_transport=stop_position AND tram=yes, public_transport=station AND tram=yes, public_transport=platform AND tram=yes, railway=tram_stop</t>
+  </si>
+  <si>
+    <t>subway stop|subway station|subway platform|subway entrance</t>
+  </si>
+  <si>
+    <t>public_transport=platform AND subway=yes, public_transport=stop_position AND subway=yes, public_transport=station AND subway=yes, railway=subway_entrance</t>
+  </si>
+  <si>
+    <t>monorail station|aerialway station|aerialway stopping location|light rail stopping location|monorail stopping location|light rail stop|light rail platform|light rail station|aerialway stop|aerialway platform|monorail platform|monorail stop</t>
+  </si>
+  <si>
+    <t>public_transport=station AND monorail=yes, public_transport=stop_position AND aerialway=yes, public_transport=stop_position AND light_rail=yes, public_transport=stop_position AND monorail=yes, public_transport=station AND light_rail=yes, public_transport=platform AND light_rail=yes, public_transport=platform AND aerialway=yes, public_transport=platform AND subway=yes, public_transport=platform AND monorail=yes</t>
+  </si>
+  <si>
+    <t>Ferry|Ferry terminal|ferry stopping location|ferry platform|ferry dock|public water transit|public water transport|marine terminal| ferry port | ferry arrival | ferry departure</t>
+  </si>
+  <si>
+    <t>amenity=ferry_terminal, public_transport=station AND ferry=yes, public_transport=stop_position AND ferry=yes, public_transport=platform AND ferry=yes</t>
+  </si>
+  <si>
+    <t>spike strip|wicket gate|sally port|stile|bump gate|wire gate|kissing gate|mororcycle barrier|railing|noise barrier|drive through gate</t>
+  </si>
+  <si>
+    <t>barrier=yes, barrier=fence AND fence_type=railing, barrier=wall AND wall=noise_barrier</t>
+  </si>
+  <si>
+    <t>Public Prosecutor's Office|attorney general, district attorney</t>
+  </si>
+  <si>
+    <t>office=government AND government=prosecutor</t>
+  </si>
+  <si>
+    <t>Notary Office</t>
+  </si>
+  <si>
+    <t>office=lawyer AND lawyer=notary</t>
+  </si>
+  <si>
+    <t>Liaison Office|diplomatic mission</t>
+  </si>
+  <si>
+    <t>office=diplomatic AND diplomatic=liaison</t>
+  </si>
+  <si>
+    <t>Consulate|consular post</t>
+  </si>
+  <si>
+    <t>office=diplomatic AND diplomatic=consulate</t>
+  </si>
+  <si>
+    <t>Embassy|foreign mission</t>
+  </si>
+  <si>
+    <t>office=diplomatic AND diplomatic=embassy, amenity=embassy</t>
+  </si>
+  <si>
+    <t>wintersports|sleigh trail|sled run|ski trail|ski touring trail|ice skating trail|ice skating ring|snowshoeing|winter hiking trail|cross-country ski trail|snowsport trail|piste|downhill ski run|snowsports half pipe|snow park|ski jump</t>
+  </si>
+  <si>
+    <t>piste:type=sleigh, piste:type=sled,piste:type=skitour, piste:type=ice_skate, piste:type=hike, piste:type=nordic, piste:type=downhill, piste:type=downhill AND man_made=piste:halfpipe, piste:type=snow_park, piste:type=ski_jump</t>
+  </si>
+  <si>
+    <t>Tourism map|public map|visitor center|public guidepost|trail marker|public information terminal|information terminal|public information board</t>
+  </si>
+  <si>
+    <t>tourism=information AND information=***any***</t>
+  </si>
+  <si>
+    <t>art gallery</t>
+  </si>
+  <si>
+    <t>tourism=gallery</t>
+  </si>
+  <si>
+    <t>public artwork|artwork|bust|statue|sculpture|art installation</t>
+  </si>
+  <si>
+    <t>tourism=artwork, tourism=artwork AND artwork_type=bust, tourism=artwork AND artwork_type=statue, tourism=artwork AND artwork_type=sculpture, tourism=artwork AND artwork_type=installation</t>
+  </si>
+  <si>
+    <t>graffiti|mural</t>
+  </si>
+  <si>
+    <t>tourism=artwork AND artwork_type=graffiti, tourism=artwork AND artwork_type=mural</t>
+  </si>
+  <si>
+    <t>campsite|camping area|camp ground|camping|backpacking site|camp pitch</t>
+  </si>
+  <si>
+    <t>tourism=camp_site, tourism=camp_pitch</t>
+  </si>
+  <si>
+    <t>wetland|Bog|Swamp|String Bog|Coastal Salt Marsh|Fen|reed bed|mangrove|marsh|wet meadow|tidal flat</t>
+  </si>
+  <si>
+    <t>natural=wetland, wetland=***any***</t>
+  </si>
+  <si>
+    <t>Oxbow Lake</t>
+  </si>
+  <si>
+    <t>water=oxbow</t>
+  </si>
+  <si>
+    <t>Dovecote|Dove house|Pigeonhole|Pigeon house|doocot|Dovecot|birdhouse</t>
+  </si>
+  <si>
+    <t>man_made=dovecote</t>
+  </si>
+  <si>
+    <t>Cross|wayside cross</t>
+  </si>
+  <si>
+    <t>man_made=cross, historic=wayside_cross</t>
+  </si>
+  <si>
+    <t>Embankment</t>
+  </si>
+  <si>
+    <t>man_made=embankment</t>
+  </si>
+  <si>
+    <t>Satellite Dish|parabolic dish|satellite communication</t>
+  </si>
+  <si>
+    <t>man_made=satellite_dish</t>
+  </si>
+  <si>
+    <t>Compass Rose|rose of the winds|public compass</t>
+  </si>
+  <si>
+    <t>man_made=compass_rose</t>
+  </si>
+  <si>
+    <t>EV Charging Point|electrical vehicle|electrical charge point| EV charging station|car charging station|charging station</t>
+  </si>
+  <si>
+    <t>man_made=charge_point</t>
+  </si>
+  <si>
+    <t>Flagpole|flag</t>
+  </si>
+  <si>
+    <t>man_made=flagpole</t>
+  </si>
+  <si>
+    <t>Beehive|apiary|beekeeper|honey farm|pollination</t>
+  </si>
+  <si>
+    <t>man_made=beehive</t>
+  </si>
+  <si>
+    <t>Street Cabinet|cable TV cabinet|telecommunications cabinet|technical box|telecom exchange</t>
+  </si>
+  <si>
+    <t>man_made=street_cabinet, telecom=exchange</t>
+  </si>
+  <si>
+    <t>Utility Pole|telephone pole|electricity pole</t>
+  </si>
+  <si>
+    <t>man_made=utility_pole</t>
+  </si>
+  <si>
+    <t>Digital Screen|video wall|public screen|display|led wall</t>
+  </si>
+  <si>
+    <t>man_made=video_wall</t>
+  </si>
+  <si>
+    <t>Tunnel Area|Tunnel|Underground passgae|underpass</t>
+  </si>
+  <si>
+    <t>man_made=tunnel</t>
+  </si>
+  <si>
+    <t>Storage Tank</t>
+  </si>
+  <si>
+    <t>man_made=storage_tank</t>
+  </si>
+  <si>
+    <t>Pagoda|buddhist tower|tiered tower</t>
+  </si>
+  <si>
+    <t>man_made=tower AND tower:type=pagoda</t>
+  </si>
+  <si>
+    <t>Bell Tower|belfry|bell gable|campanile|klockstapel</t>
+  </si>
+  <si>
+    <t>man_made=tower AND tower:type=bell_tower</t>
+  </si>
+  <si>
+    <t>Cosmetics Store|make up shop|make-up shop</t>
+  </si>
+  <si>
+    <t>shop=cosmetics</t>
+  </si>
+  <si>
+    <t>Seafood Shop|fish shop</t>
+  </si>
+  <si>
+    <t>shop=seafood</t>
+  </si>
+  <si>
+    <t>Furniture Store|interior shop</t>
+  </si>
+  <si>
+    <t>shop=furniture</t>
+  </si>
+  <si>
+    <t>Tailor</t>
+  </si>
+  <si>
+    <t>shop=tailor</t>
+  </si>
+  <si>
+    <t>entrance|exit</t>
+  </si>
+  <si>
+    <t>building=entrance</t>
+  </si>
+  <si>
+    <t>Yurt|Ger</t>
+  </si>
+  <si>
+    <t>building=ger</t>
+  </si>
+  <si>
+    <t>Cabin</t>
+  </si>
+  <si>
+    <t>building=cabin</t>
+  </si>
+  <si>
+    <t>Bungalow</t>
+  </si>
+  <si>
+    <t>building=bungalow</t>
+  </si>
+  <si>
+    <t>Allotment House</t>
+  </si>
+  <si>
+    <t>building=allotment_house</t>
+  </si>
+  <si>
+    <t>Boathouse</t>
+  </si>
+  <si>
+    <t>building=boathouse</t>
+  </si>
+  <si>
+    <t>Slaughterhouse|abattoir|butchery|killing house</t>
+  </si>
+  <si>
+    <t>industrial=slaughterhouse</t>
+  </si>
+  <si>
+    <t>Scrap Yard|junk yard|junk shop|scrap heap|wreck yard</t>
+  </si>
+  <si>
+    <t>industrial=scrap_yard</t>
+  </si>
+  <si>
+    <t>Fire Pit|bonfire|campfire|fire place</t>
+  </si>
+  <si>
+    <t>leisure=firepit</t>
+  </si>
+  <si>
+    <t>trampoline park</t>
+  </si>
+  <si>
+    <t>leisure=trampoline_park</t>
+  </si>
+  <si>
+    <t>chess table|public chess board|public chess</t>
+  </si>
+  <si>
+    <t>leisure=picnic_table AND sport=chess, sport=chess</t>
+  </si>
+  <si>
+    <t>resort|sanatorium|vacation resort</t>
+  </si>
+  <si>
+    <t>leisure=resort</t>
+  </si>
+  <si>
+    <t>public fitness|public exercise|outdoor fitness|outdoor exercise</t>
+  </si>
+  <si>
+    <t>leisure=fitness_station</t>
+  </si>
+  <si>
+    <t>padel court|padel</t>
+  </si>
+  <si>
+    <t>sport=padel</t>
+  </si>
+  <si>
+    <t>boules|bocce court|pétanque|pétangue|petanque|bocce|jeu de boules</t>
+  </si>
+  <si>
+    <t>sport=boules</t>
+  </si>
+  <si>
+    <t>skate park|bmx|skateboarding|skatepark</t>
+  </si>
+  <si>
+    <t>sport=skateboard</t>
+  </si>
+  <si>
+    <t>rugby league field|rugby union field|rugby field</t>
+  </si>
+  <si>
+    <t>sport=rugby_league, sport=rugby_union</t>
+  </si>
+  <si>
+    <t>australian football field|AFL</t>
+  </si>
+  <si>
+    <t>sport=australian_football</t>
+  </si>
+  <si>
+    <t>bowling green</t>
+  </si>
+  <si>
+    <t>sport=bowls</t>
+  </si>
+  <si>
+    <t>four square court|4square|4 square</t>
+  </si>
+  <si>
+    <t>sport=four_square</t>
+  </si>
+  <si>
+    <t>ping pong table|table tennis</t>
+  </si>
+  <si>
+    <t>sport=table_tennis</t>
+  </si>
+  <si>
+    <t>cricket field|cricket</t>
+  </si>
+  <si>
+    <t>sport=cricket</t>
+  </si>
+  <si>
+    <t>team handball court|handball</t>
+  </si>
+  <si>
+    <t>sport=handball, sport=american_handball</t>
+  </si>
+  <si>
+    <t>beach volleyball court|beach volleyball</t>
+  </si>
+  <si>
+    <t>sport=beachvolleyball</t>
+  </si>
+  <si>
+    <t>shooting Range|firing range|gun range|shooting gallery|gun practice|shooting practice|target practice</t>
+  </si>
+  <si>
+    <t>sport=shooting</t>
+  </si>
+  <si>
+    <t>hammer throw ring|hammer throw</t>
+  </si>
+  <si>
+    <t>sport=athletics AND athletics=hammer_throw</t>
+  </si>
+  <si>
+    <t>shot put ring|shot put pit</t>
+  </si>
+  <si>
+    <t>sport=athletics AND athletics=shot_put</t>
+  </si>
+  <si>
+    <t>paintball field</t>
+  </si>
+  <si>
+    <t>sport=paintball</t>
+  </si>
+  <si>
+    <t>funnel ball court</t>
+  </si>
+  <si>
+    <t>sport=funnel_ball</t>
+  </si>
+  <si>
+    <t>softball field</t>
+  </si>
+  <si>
+    <t>sport=softball</t>
+  </si>
+  <si>
+    <t>american football field</t>
+  </si>
+  <si>
+    <t>sport=american_football</t>
+  </si>
+  <si>
+    <t>archery range|bow and arrow|crossbow|bow shooting</t>
+  </si>
+  <si>
+    <t>sport=archery</t>
+  </si>
+  <si>
+    <t>netball</t>
+  </si>
+  <si>
+    <t>sport=netball</t>
+  </si>
+  <si>
+    <t>tetherball|swingball</t>
+  </si>
+  <si>
+    <t>sport=tetherball</t>
+  </si>
+  <si>
+    <t>field hockey</t>
+  </si>
+  <si>
+    <t>sport=field_hockey</t>
+  </si>
+  <si>
+    <t>shuffleboard</t>
+  </si>
+  <si>
+    <t>sport=shuffleboard</t>
+  </si>
+  <si>
+    <t>gaga pit</t>
+  </si>
+  <si>
+    <t>sport=gaga</t>
+  </si>
+  <si>
+    <t>badminton</t>
+  </si>
+  <si>
+    <t>sport=badminton</t>
+  </si>
+  <si>
+    <t>volleyball</t>
+  </si>
+  <si>
+    <t>sport=volleyball</t>
+  </si>
+  <si>
+    <t>pickleball court</t>
+  </si>
+  <si>
+    <t>sport=pickleball</t>
+  </si>
+  <si>
+    <t>yoga|yoga studio|asanas|meditation center|meditation studio</t>
+  </si>
+  <si>
+    <t>sport=yoga</t>
+  </si>
+  <si>
+    <t>climbing gym|climbing center|boulder center|bouldering|rock climbing|rock gym|climbing wall|boulder gym</t>
+  </si>
+  <si>
+    <t>sport=climbing, climbing=boulder, climbing:boulder=yes</t>
+  </si>
+  <si>
+    <t>adventure park|obstacle course|rope climbing</t>
+  </si>
+  <si>
+    <t>sport=climbing_adventure</t>
+  </si>
+  <si>
+    <t>community garden|co-op garden|collective garden|communal garden</t>
+  </si>
+  <si>
+    <t>leisure=garden AND garden:type=community</t>
+  </si>
+  <si>
+    <t>botanical garden|rare plants|botanic garden</t>
+  </si>
+  <si>
+    <t>leisure=garden AND garden:type=botanical</t>
+  </si>
+  <si>
+    <t>residential garden|back garden|back yard|domestic garden|front garden|front yard|private garden</t>
+  </si>
+  <si>
+    <t>leisure=garden AND garden:type=residential</t>
+  </si>
+  <si>
+    <t>traffic calming|speed bump|speed hump|speed table|traffic island|speed cushion|traffic choker|traffic rumble strip|chicane|traffic chicane</t>
+  </si>
+  <si>
+    <t>traffic_calming=***any***</t>
+  </si>
+  <si>
+    <t>smoking area|smokers' area</t>
+  </si>
+  <si>
+    <t>amenity=smoking_area</t>
+  </si>
+  <si>
+    <t>dojo|martial arts|dojang</t>
+  </si>
+  <si>
+    <t>amenity=dojo</t>
+  </si>
+  <si>
+    <t>coworking space|coworking place|coworking office</t>
+  </si>
+  <si>
+    <t>amenity=coworking_space</t>
+  </si>
+  <si>
+    <t>permanent polling place|ballot box|ballot drop|polling place|voting booth|voting machine|polling station</t>
+  </si>
+  <si>
+    <t>amenity=polling_station</t>
+  </si>
+  <si>
+    <t>shisha lounge|hookah lounge|waterpipe|nargile</t>
+  </si>
+  <si>
+    <t>amenity=hookah_lounge</t>
+  </si>
+  <si>
+    <t>second hand shop|2nd hand shop</t>
+  </si>
+  <si>
+    <t>amenity=recycling AND recycling:electrical_items=yes</t>
+  </si>
+  <si>
+    <t>green waste|biodegradable waste|biological waste|compost</t>
+  </si>
+  <si>
+    <t>amenity=recycling AND recycling:green_waste=yes</t>
+  </si>
+  <si>
+    <t>abortion clinic</t>
+  </si>
+  <si>
+    <t>healthcare:speciality=abortion</t>
+  </si>
+  <si>
+    <t>transit shelter|public transport shelter</t>
+  </si>
+  <si>
+    <t>amenity=shelter AND shelter_type=public_transport</t>
+  </si>
+  <si>
+    <t>nightclub|dance club|dancing|disco|discotheque|night club</t>
+  </si>
+  <si>
+    <t>amenity=nightclub</t>
+  </si>
+  <si>
+    <t>place of worship|house of god|house of worship</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship, building=cathedral, building=chapel, building=church, building=mosque, building=shrine, building=synagogue, building=temple</t>
+  </si>
+  <si>
+    <t>religion</t>
+  </si>
+  <si>
+    <t>religion=***example***</t>
+  </si>
+  <si>
+    <t>denomination</t>
+  </si>
+  <si>
+    <t>denomination=***example***</t>
+  </si>
+  <si>
+    <t>Sikh Temple</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=sikh</t>
+  </si>
+  <si>
+    <t>Shinto Shrine</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=shinto</t>
+  </si>
+  <si>
+    <t>Jewish Synagogue|synagogue|shul|jewish temple|jewish house of worship</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=jewish, building=synagogue</t>
+  </si>
+  <si>
+    <t>Taoist Temple</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=taoist</t>
+  </si>
+  <si>
+    <t>Christian Church</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship  AND religion=christian</t>
+  </si>
+  <si>
+    <t>Muslim Mosque</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=muslim, building=mosque</t>
+  </si>
+  <si>
+    <t>Minaret|Muezzin</t>
+  </si>
+  <si>
+    <t>man_made=tower AND tower:type=minaret</t>
+  </si>
+  <si>
+    <t>Buddhist Temple</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship  AND religion=buddhist</t>
+  </si>
+  <si>
+    <t>Hindu Temple</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=hindu</t>
+  </si>
+  <si>
+    <t>Kingdom Hall of Jehovah's Witnesses</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=christian AND denomination=jehovahs_witness</t>
+  </si>
+  <si>
+    <t>La Luz del Mundo Temple</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=christian AND denomination=la_luz_del_mundo</t>
+  </si>
+  <si>
+    <t>Quaker Friends Meeting House</t>
+  </si>
+  <si>
+    <t>amenity=place_of_worship AND religion=christian AND denomination=quaker</t>
+  </si>
+  <si>
+    <t>manhole</t>
+  </si>
+  <si>
+    <t>manhole=***any***</t>
+  </si>
+  <si>
+    <t>lighting mast|flood light|stadium lights|stadium lighting</t>
+  </si>
+  <si>
+    <t>man_made=mast AND tower:type=lighting</t>
+  </si>
+  <si>
+    <t>water tank|cistern|water tower</t>
+  </si>
+  <si>
+    <t>man_made=storage_tank AND content=water, man_made=water_tower, building=water_tower, emergency=water_tank</t>
+  </si>
+  <si>
+    <t>communication mast|broadcast tower|communication antenna|cell phone tower|mobile phone mast|radio broadcast mast|radio tower|transmission tower|tv mast|tv tower|communication tower|cell tower</t>
+  </si>
+  <si>
+    <t>man_made=communications_tower, man_made=mast AND tower:type=communication, man_made=tower AND tower:type=communication</t>
+  </si>
+  <si>
+    <t>radio telescope|ground station|radio dish|radio antenna</t>
+  </si>
+  <si>
+    <t>man_made=telescope, telescope:type=radio</t>
+  </si>
+  <si>
+    <t>optical telescope|refracting telescope|reflecting telescope</t>
+  </si>
+  <si>
+    <t>man_made=telescope, telescope:type=optical</t>
+  </si>
+  <si>
+    <t>crane|gantry crane|portal crane|overhead crane|gantry</t>
+  </si>
+  <si>
+    <t>man_made=crane AND crane:type=***any***, man_made=gantry</t>
+  </si>
+  <si>
+    <t>postal relay box|post relay box</t>
+  </si>
+  <si>
+    <t>man_made=street_cabinet AND street_cabinet=postal_service</t>
+  </si>
+  <si>
+    <t>traffic monitoring cabinet|traffic count|traffic count box|vehicle counting</t>
+  </si>
+  <si>
+    <t>man_made=street_cabinet AND street_cabinet=traffic_monitoring</t>
+  </si>
+  <si>
+    <t>first aid kit|med kit|medkit</t>
+  </si>
+  <si>
+    <t>emergency=first_aid_kit</t>
+  </si>
+  <si>
+    <t>lifeboat|marine rescue|boat rescue|lifeboat station</t>
+  </si>
+  <si>
+    <t>emergency=water_rescue</t>
+  </si>
+  <si>
+    <t>Wi-Fi Hotspot|wi-fi|public wifi|hotspot</t>
+  </si>
+  <si>
+    <t>internet_access=wlan</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>man_made=antenna</t>
+  </si>
+  <si>
+    <t>Courtyard|yard</t>
+  </si>
+  <si>
+    <t>man_made=courtyard</t>
+  </si>
+  <si>
+    <t>Torii|japanese gate|Shinto gate</t>
+  </si>
+  <si>
+    <t>man_made=torii</t>
+  </si>
+  <si>
+    <t>Obelisk</t>
+  </si>
+  <si>
+    <t>man_made=obelisk</t>
+  </si>
+  <si>
+    <t>Water Works</t>
+  </si>
+  <si>
+    <t>man_made=water_works</t>
+  </si>
+  <si>
+    <t>Beacon</t>
+  </si>
+  <si>
+    <t>man_made=beacon</t>
+  </si>
+  <si>
+    <t>Wind Turbine|aerorotor</t>
+  </si>
+  <si>
+    <t>power=generator AND generator:source=wind, generator:method=wind_turbine, plant:method=wind_turbine, generator:type=wind_turbine</t>
+  </si>
+  <si>
+    <t>windmill|wind pump</t>
+  </si>
+  <si>
+    <t>man_made=windmill, man_made=windpump</t>
+  </si>
+  <si>
+    <t>Nuclear Reactor</t>
+  </si>
+  <si>
+    <t>power=generator AND generator:source=nuclear, power=generator AND generator:method=fission</t>
+  </si>
+  <si>
+    <t>Water Turbine|water dam|hydroelectricity</t>
+  </si>
+  <si>
+    <t>power=generator AND generator:source=hydro</t>
+  </si>
+  <si>
+    <t>Solar Panel|photovoltaic|PV|sunlight energy|solar power plant|solar energy plant</t>
+  </si>
+  <si>
+    <t>power=generator AND generator:method=photovoltaic, power=plant AND plant:source=solar</t>
+  </si>
+  <si>
+    <t>Wind Farm|offshore wind|wind park|wind power plant|wind energy plant</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=wind</t>
+  </si>
+  <si>
+    <t>Waste Incineration Power Plant|garbage incinerator</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=waste</t>
+  </si>
+  <si>
+    <t>Coal-Fired Power Plant|coal fired energy plant</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=coal</t>
+  </si>
+  <si>
+    <t>Nuclear Power Plant|atomic power plant|nuclear energy plant</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=nuclear</t>
+  </si>
+  <si>
+    <t>Cooling Tower</t>
+  </si>
+  <si>
+    <t>man_made=tower AND tower:type=cooling</t>
+  </si>
+  <si>
+    <t>Hydroelectric Power Station|water power plant|tidal power plant|hydro power plant</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=hydro</t>
+  </si>
+  <si>
+    <t>Oil-Fired Power Plant|oil power station</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=oil</t>
+  </si>
+  <si>
+    <t>Gas-Fired Power Plant|gas power station</t>
+  </si>
+  <si>
+    <t>power=plant AND plant:source=gas</t>
+  </si>
+  <si>
+    <t>Parking Ticket Vending Machine|parking ticket</t>
+  </si>
+  <si>
+    <t>amenity=vending_machine AND vending=parking_tickets</t>
+  </si>
+  <si>
+    <t>Cycling track|running track|athletics track</t>
+  </si>
+  <si>
+    <t>leisure=track AND sport=cycling, leisure=track AND sport=running, leisure=track AND sport=athletics, sport=athletics</t>
+  </si>
+  <si>
+    <t>Horse Racetrack|equestrian race track|horse racing</t>
+  </si>
+  <si>
+    <t>sport=horse_racing</t>
+  </si>
+  <si>
+    <t>Advertising Totem|Poster Box|Billboard|Notice Board|advertising board|advertising column|advertising screen|advertising sign|advertising tarp|wall painting</t>
+  </si>
+  <si>
+    <t>advertising=***any***</t>
+  </si>
+  <si>
+    <t>Destination Sign</t>
+  </si>
+  <si>
+    <t>street_sign=destination_sign</t>
+  </si>
+  <si>
+    <t>Hiking route|walking route|outdoor sports|bicycle route</t>
+  </si>
+  <si>
+    <t>route=hiking, route=bicyle, route=walking</t>
+  </si>
+  <si>
+    <t>public transport routes | bus route | tram route |metro route</t>
+  </si>
+  <si>
+    <t>route=bus, route= train, route= ferry, route=tram, route= trolleybus, route=subway</t>
+  </si>
+  <si>
+    <t>Garden Center|flower store</t>
+  </si>
+  <si>
+    <t>shop=garden_centre, shop=flowers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer Store </t>
+  </si>
+  <si>
+    <t>shop=computer</t>
+  </si>
+  <si>
+    <t>rental shop</t>
+  </si>
+  <si>
+    <t>shop=rental</t>
+  </si>
+  <si>
+    <t>Chocolate Store|candy store</t>
+  </si>
+  <si>
+    <t>Outdoor store</t>
+  </si>
+  <si>
+    <t>shop=outdoor</t>
+  </si>
+  <si>
+    <t>Funeral Home|morgue|crematorium|mortuary</t>
+  </si>
+  <si>
+    <t>shop=funeral_directors, amenity=mortuary</t>
+  </si>
+  <si>
+    <t>Storage Rental</t>
+  </si>
+  <si>
+    <t>shop=storage_rental</t>
+  </si>
+  <si>
+    <t>Erotic Store | sex shop</t>
+  </si>
+  <si>
+    <t>shop=erotic, shop=sex</t>
+  </si>
+  <si>
+    <t>Motorcycle Repair Shop</t>
+  </si>
+  <si>
+    <t>shop=motorcycle_repair</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>shop=butcher</t>
+  </si>
+  <si>
+    <t>Arts &amp; Crafts Store</t>
+  </si>
+  <si>
+    <t>shop=craft</t>
+  </si>
+  <si>
+    <t>Furnishing Store|carpet|curtains|mattress|luggage</t>
+  </si>
+  <si>
+    <t>shop=bathroom_furnishing, shop=carpet, shop=curtains, shop=bed, shop=luggage</t>
+  </si>
+  <si>
+    <t>house number|building number</t>
+  </si>
+  <si>
+    <t>addr:housenumber=***example***</t>
+  </si>
+  <si>
+    <t>roof material</t>
+  </si>
+  <si>
+    <t>roof:material=***example***</t>
+  </si>
+  <si>
+    <t>elevator</t>
+  </si>
+  <si>
+    <t>elevator=yes</t>
+  </si>
+  <si>
+    <t>pet shop|animal shop</t>
+  </si>
+  <si>
+    <t>shop=pet, shop=pet_grooming</t>
+  </si>
+  <si>
+    <t>stadium|stadion|pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leisure=stadium, leisure=pitch, building=stadium, stadium=football, stadium=soccer, </t>
+  </si>
+  <si>
+    <t>sport</t>
+  </si>
+  <si>
+    <t>sport=***example***</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>shop=***any***</t>
+  </si>
+  <si>
+    <t>school|highschool|elementary school|school building|language school|music school|learning center|preparatory school|prep school</t>
+  </si>
+  <si>
+    <t>car rental|car sharing parking lot|Car sharing spots|car sharing place|hire car|car pool|car pooling station</t>
+  </si>
+  <si>
+    <t>parking spaces|parking spots|parking|parking area|Parking lots|parking zone|parking aisle|street side parking| parking space|parking spot| parking slot| parking place| parking stall|accessible parking space</t>
+  </si>
+  <si>
+    <t>community centre|rec center|recreation center|community hall|activity center|neighborhood center|cultural center|civic centre</t>
+  </si>
+  <si>
+    <t>amenity=community_centre, amenity=social_centre</t>
+  </si>
+  <si>
+    <t>conference centre|convention center|meeting venue|conference facility|symposium center|exhibition center|trade fair|trade fair center|congress center</t>
+  </si>
+  <si>
+    <t>TV studio|radio studio|recording studio|production studio|sound studio|music studio|audio lab|broadcasting studio|news studio|film studio</t>
+  </si>
+  <si>
+    <t>amenity=toilets, building=toilets, toilets=yes</t>
+  </si>
+  <si>
+    <t>refugee site| refugee camp| refugee center| refugee settlement| refugee shelter| displaced persons camp</t>
+  </si>
+  <si>
+    <t>amenity=refugee_site</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>fire tower|observation tower|lookout tower</t>
+  </si>
+  <si>
+    <t>man_made=tower AND tower:type=observation</t>
+  </si>
+  <si>
+    <t>lifeguard spot</t>
+  </si>
+  <si>
+    <t>speed camera</t>
+  </si>
+  <si>
+    <t>highway=street_lamp</t>
+  </si>
+  <si>
+    <t>Military Trench|war trench</t>
+  </si>
+  <si>
+    <t>winter sports</t>
+  </si>
+  <si>
+    <t>stadium|stadium building</t>
+  </si>
+  <si>
+    <t>leisure=stadium, building=stadium</t>
+  </si>
+  <si>
+    <t>estate agent</t>
+  </si>
+  <si>
+    <t>politician's office</t>
+  </si>
+  <si>
+    <t>office of a political party</t>
+  </si>
+  <si>
     <t>power tower|power pole</t>
-  </si>
-  <si>
-    <t>power=tower, power=pole</t>
-  </si>
-  <si>
-    <t>abandoned|disused railway track|decommissioned railroad|Abandoned train track|disused railway|extinct line|deserted train track</t>
-  </si>
-  <si>
-    <t>railway=abandoned, railway=disused</t>
-  </si>
-  <si>
-    <t>railway under construction|railway repair</t>
-  </si>
-  <si>
-    <t>railway=construction</t>
-  </si>
-  <si>
-    <t>railroad track|Railway track|train track|train line</t>
-  </si>
-  <si>
-    <t>railway=rail, railway=light_rail, railway=miniature, railway=narrow_gauge, railway=subway, railway=tram, railway=route</t>
-  </si>
-  <si>
-    <t>high-speed train track|high speed train track</t>
-  </si>
-  <si>
-    <t>railway=rail AND highspeed=yes</t>
-  </si>
-  <si>
-    <t>tram track|tram|subway|light rail|subway track|metro|underground|tube|rapid transit</t>
-  </si>
-  <si>
-    <t>railway=subway, railway=tram, railway=light_rail</t>
-  </si>
-  <si>
-    <t>railway bridge|railroad viaduct|train bridge|railroad bridge|trestle bridge</t>
-  </si>
-  <si>
-    <t>railway=***any*** AND bridge=yes</t>
-  </si>
-  <si>
-    <t>railway cutting|submerged railway|sunken railway|under-level railway</t>
-  </si>
-  <si>
-    <t>cutting=yes</t>
-  </si>
-  <si>
-    <t>railway tunnel|train tunnel|metro tunnel|railway underpass|subway tunnel|railroad tunnel</t>
-  </si>
-  <si>
-    <t>railway=***any*** AND tunnel=yes</t>
-  </si>
-  <si>
-    <t>railway crossing|level crossing|grade crossing|pedestrian railway crossing</t>
-  </si>
-  <si>
-    <t>railway=crossing, railway=level_crossing, railway=tram_level_crossing, railway=railway_crossing</t>
-  </si>
-  <si>
-    <t>railway signal|railroad signal|railway light|train signal|trackside signal|railroad light|train signaling lights</t>
-  </si>
-  <si>
-    <t>railway=signal</t>
-  </si>
-  <si>
-    <t>railway switch|track switch|railroad switch|train switch|train crossover</t>
-  </si>
-  <si>
-    <t>railway=switch</t>
-  </si>
-  <si>
-    <t>turntable|rotating train platform|revolving train platform</t>
-  </si>
-  <si>
-    <t>railway=turntable</t>
-  </si>
-  <si>
-    <t>alcohol shop</t>
-  </si>
-  <si>
-    <t>shop=alcohol</t>
-  </si>
-  <si>
-    <t>bakery</t>
-  </si>
-  <si>
-    <t>shop=bakery</t>
-  </si>
-  <si>
-    <t>department store|large store</t>
-  </si>
-  <si>
-    <t>shop=department_store</t>
-  </si>
-  <si>
-    <t>mall|shopping centre</t>
-  </si>
-  <si>
-    <t>shop=mall</t>
-  </si>
-  <si>
-    <t>supermarket|discount|wholesale|discounter</t>
-  </si>
-  <si>
-    <t>shop=supermarket, building=supermarket, shop=discounter, shop=wholesale</t>
-  </si>
-  <si>
-    <t>clothes shop|clothing store|fashion store|boutique|fashion accessories</t>
-  </si>
-  <si>
-    <t>shop=clothes, shop=fashion, shop=boutique, shop=fashion_accessories</t>
-  </si>
-  <si>
-    <t>fabric shop</t>
-  </si>
-  <si>
-    <t>shop=fabric</t>
-  </si>
-  <si>
-    <t>jewelry shop</t>
-  </si>
-  <si>
-    <t>shop=jewelry</t>
-  </si>
-  <si>
-    <t>shoe shop</t>
-  </si>
-  <si>
-    <t>shop=shoes</t>
-  </si>
-  <si>
-    <t>charity shop</t>
-  </si>
-  <si>
-    <t>shop=charity</t>
-  </si>
-  <si>
-    <t>second hand shop</t>
-  </si>
-  <si>
-    <t>shop=second_hand</t>
-  </si>
-  <si>
-    <t>beauty shop|nail salon</t>
-  </si>
-  <si>
-    <t>shop=beauty</t>
-  </si>
-  <si>
-    <t>hairdresser</t>
-  </si>
-  <si>
-    <t>shop=hairdresser</t>
-  </si>
-  <si>
-    <t>medical supply store</t>
-  </si>
-  <si>
-    <t>shop=medical_supply</t>
-  </si>
-  <si>
-    <t>tattoo shop|tattoo parlour</t>
-  </si>
-  <si>
-    <t>shop=tattoo</t>
-  </si>
-  <si>
-    <t>doityourself shop|DIY shop</t>
-  </si>
-  <si>
-    <t>shop=doityourself</t>
-  </si>
-  <si>
-    <t>florist</t>
-  </si>
-  <si>
-    <t>shop=florist</t>
-  </si>
-  <si>
-    <t>electronics shop</t>
-  </si>
-  <si>
-    <t>shop=electronics</t>
-  </si>
-  <si>
-    <t>mobile phone shop</t>
-  </si>
-  <si>
-    <t>shop=mobile_phone</t>
-  </si>
-  <si>
-    <t>bicycle shop</t>
-  </si>
-  <si>
-    <t>shop=bicycle</t>
-  </si>
-  <si>
-    <t>boat shop</t>
-  </si>
-  <si>
-    <t>shop=boat</t>
-  </si>
-  <si>
-    <t>car shop|car repair shop|car repair</t>
-  </si>
-  <si>
-    <t>shop=car, shop=car_repair, shop=car_parts</t>
-  </si>
-  <si>
-    <t>fuel shop</t>
-  </si>
-  <si>
-    <t>shop=fuel</t>
-  </si>
-  <si>
-    <t>hunting shop</t>
-  </si>
-  <si>
-    <t>shop=hunting</t>
-  </si>
-  <si>
-    <t>military surplus shop</t>
-  </si>
-  <si>
-    <t>shop=military_surplus</t>
-  </si>
-  <si>
-    <t>motorcycle shop|motorcycle rental</t>
-  </si>
-  <si>
-    <t>shop=motorcycle, amenity=motorcycle_rental</t>
-  </si>
-  <si>
-    <t>sports shop| sport shop</t>
-  </si>
-  <si>
-    <t>shop=sports</t>
-  </si>
-  <si>
-    <t>art store|art shop</t>
-  </si>
-  <si>
-    <t>shop=art</t>
-  </si>
-  <si>
-    <t>Antique Shop|antiques shop|vintage store|antiques store|antiquities shop</t>
-  </si>
-  <si>
-    <t>shop=antiques</t>
-  </si>
-  <si>
-    <t>camera shop</t>
-  </si>
-  <si>
-    <t>shop=camera</t>
-  </si>
-  <si>
-    <t>music shop | instrument shop</t>
-  </si>
-  <si>
-    <t>shop=music, shop=musical_instrument</t>
-  </si>
-  <si>
-    <t>book shop|book store</t>
-  </si>
-  <si>
-    <t>shop=books</t>
-  </si>
-  <si>
-    <t>lottery shop</t>
-  </si>
-  <si>
-    <t>shop=lottery</t>
-  </si>
-  <si>
-    <t>laundry shop|laundry place|self service laundry</t>
-  </si>
-  <si>
-    <t>shop=laundry</t>
-  </si>
-  <si>
-    <t>travel agency</t>
-  </si>
-  <si>
-    <t>shop=travel_agency</t>
-  </si>
-  <si>
-    <t>weapon shop</t>
-  </si>
-  <si>
-    <t>shop=weapons</t>
-  </si>
-  <si>
-    <t>vacant shop</t>
-  </si>
-  <si>
-    <t>shop=vacant</t>
-  </si>
-  <si>
-    <t>baseball facility|baseball field</t>
-  </si>
-  <si>
-    <t>sport=baseball</t>
-  </si>
-  <si>
-    <t>basketball facility|basketball field</t>
-  </si>
-  <si>
-    <t>sport=basketball</t>
-  </si>
-  <si>
-    <t>golf facility|golf course</t>
-  </si>
-  <si>
-    <t>sport=golf, golf=***any***, leisure=golf_course</t>
-  </si>
-  <si>
-    <t>mini golf|miniature golf|putt-putt|crazy golf</t>
-  </si>
-  <si>
-    <t>leisure=miniature_golf</t>
-  </si>
-  <si>
-    <t>disc golf|disc golf course</t>
-  </si>
-  <si>
-    <t>disc_golf=***any***, leisure=disc_golf_course</t>
-  </si>
-  <si>
-    <t>Bowling Alley|bowling center</t>
-  </si>
-  <si>
-    <t>leisure=bowling_alley</t>
-  </si>
-  <si>
-    <t>ice skating field|ice skating hall|ice hockey</t>
-  </si>
-  <si>
-    <t>sport=ice_skating, sport=ice_hockey</t>
-  </si>
-  <si>
-    <t>sports facility|sports hall|sports center|sports club|athletics club|sporting club|sports association|sports society</t>
-  </si>
-  <si>
-    <t>sport=multi, building=sports_hall, club=sport, leisure=sports_hall</t>
-  </si>
-  <si>
-    <t>soccer field| soccer hall|soccer facility</t>
-  </si>
-  <si>
-    <t>sport=soccer</t>
-  </si>
-  <si>
-    <t>tennis court|tennis facility</t>
-  </si>
-  <si>
-    <t>sport=tennis</t>
-  </si>
-  <si>
-    <t>data center</t>
-  </si>
-  <si>
-    <t>telecom=data_center</t>
-  </si>
-  <si>
-    <t>alpine hut</t>
-  </si>
-  <si>
-    <t>tourism=alpine_hut</t>
-  </si>
-  <si>
-    <t>aquarium</t>
-  </si>
-  <si>
-    <t>tourism=aquarium</t>
-  </si>
-  <si>
-    <t>tourist attraction</t>
-  </si>
-  <si>
-    <t>tourism=attraction</t>
-  </si>
-  <si>
-    <t>parking lot for campers|caravan site|parking area for motorhomes</t>
-  </si>
-  <si>
-    <t>tourism=caravan_site</t>
-  </si>
-  <si>
-    <t>chalet</t>
-  </si>
-  <si>
-    <t>tourism=chalet</t>
-  </si>
-  <si>
-    <t>guest house</t>
-  </si>
-  <si>
-    <t>tourism=guest_house</t>
-  </si>
-  <si>
-    <t>hostel</t>
-  </si>
-  <si>
-    <t>tourism=hostel</t>
-  </si>
-  <si>
-    <t>hotel</t>
-  </si>
-  <si>
-    <t>tourism=hotel, building=hotel</t>
-  </si>
-  <si>
-    <t>tourist information</t>
-  </si>
-  <si>
-    <t>tourism=information</t>
-  </si>
-  <si>
-    <t>motel</t>
-  </si>
-  <si>
-    <t>tourism=motel, building=motel</t>
-  </si>
-  <si>
-    <t>museum</t>
-  </si>
-  <si>
-    <t>tourism=museum, building=museum</t>
-  </si>
-  <si>
-    <t>picnic site|picnic table|picnic shelter|picnic pavilion</t>
-  </si>
-  <si>
-    <t>tourism=picnic_site, leisure=picnic_table, amenity=shelter AND shelter_type=picnic_shelter</t>
-  </si>
-  <si>
-    <t>amusement park|carnival|fairground|funfair|festival ground|Fair|theme park</t>
-  </si>
-  <si>
-    <t>tourism=theme_park, landuse=fairground, landuse=recreation_ground, recreation_ground=showground, amenity=festival_grounds, leisure=festival_grounds, attraction=big_wheel AND attraction=roller_coaster</t>
-  </si>
-  <si>
-    <t>viewpoint|view point</t>
-  </si>
-  <si>
-    <t>tourism=viewpoint</t>
-  </si>
-  <si>
-    <t>zoo</t>
-  </si>
-  <si>
-    <t>tourism=zoo</t>
-  </si>
-  <si>
-    <t>canal|stream|river|channelstream area|creek|brook|watercourse|surge</t>
-  </si>
-  <si>
-    <t>water=river, water=stream, water=canal, waterway=river, waterway=stream, waterway=canal, water=oxbow</t>
-  </si>
-  <si>
-    <t>ditch</t>
-  </si>
-  <si>
-    <t>water=ditch, waterway=drain, waterway=ditch, barrier=ditch</t>
-  </si>
-  <si>
-    <t>lock for boats|lock</t>
-  </si>
-  <si>
-    <t>water=lock</t>
-  </si>
-  <si>
-    <t>lake|pond</t>
-  </si>
-  <si>
-    <t>water=lake, water=pond, landuse=pond</t>
-  </si>
-  <si>
-    <t>basin|reservoir|salt pond|water reservoir|wastewater basin</t>
-  </si>
-  <si>
-    <t>water=basin, landuse=basin, landuse=reservoir, landuse=salt_pond, water=basin, water=reservoir, man_made=reservoir_covered, water=wastewater</t>
-  </si>
-  <si>
-    <t>lagoon</t>
-  </si>
-  <si>
-    <t>water=lagoon</t>
-  </si>
-  <si>
-    <t>moat</t>
-  </si>
-  <si>
-    <t>water=moat</t>
-  </si>
-  <si>
-    <t>wastewater</t>
-  </si>
-  <si>
-    <t>water=wastewater</t>
-  </si>
-  <si>
-    <t>ship repair dock|dry dock|boatyard|boat storage</t>
-  </si>
-  <si>
-    <t>waterway=dock, waterway=boatyard, amenity=boat_storage</t>
-  </si>
-  <si>
-    <t>dam</t>
-  </si>
-  <si>
-    <t>waterway=dam</t>
-  </si>
-  <si>
-    <t>weir</t>
-  </si>
-  <si>
-    <t>waterway=weir</t>
-  </si>
-  <si>
-    <t>waterfall</t>
-  </si>
-  <si>
-    <t>waterway=waterfall</t>
-  </si>
-  <si>
-    <t>boat fuelling station|ship fuelling station</t>
-  </si>
-  <si>
-    <t>waterway=fuel</t>
-  </si>
-  <si>
-    <t>street name</t>
-  </si>
-  <si>
-    <t>addr:street~***any***</t>
-  </si>
-  <si>
-    <t>name|brand|brand name</t>
-  </si>
-  <si>
-    <t>name~***example***, brand~***example***</t>
-  </si>
-  <si>
-    <t>toll road</t>
-  </si>
-  <si>
-    <t>toll=yes</t>
-  </si>
-  <si>
-    <t>city limit sign</t>
-  </si>
-  <si>
-    <t>traffic_sign=city_limit</t>
-  </si>
-  <si>
-    <t>living street|neighbourhood street|residential road</t>
-  </si>
-  <si>
-    <t>highway=residential, highway=living_street, highway=service</t>
-  </si>
-  <si>
-    <t>divided highway|dual carriageway road|Dual carriageway</t>
-  </si>
-  <si>
-    <t>dual_carriageway=yes, area:highway=traffic_island</t>
-  </si>
-  <si>
-    <t>slip course|slip track|slip training</t>
-  </si>
-  <si>
-    <t>leisure=slipway</t>
-  </si>
-  <si>
-    <t>monorail|single rail system|monorail track</t>
-  </si>
-  <si>
-    <t>railway=monorail</t>
-  </si>
-  <si>
-    <t>funicular|cable railway|incline railway</t>
-  </si>
-  <si>
-    <t>railway=funicular</t>
-  </si>
-  <si>
-    <t>Train yard|railyard|rail yard|train depot</t>
-  </si>
-  <si>
-    <t>landuse=depot, service=yard, landuse=railway</t>
-  </si>
-  <si>
-    <t>inlet|Estuary|baymouth bar</t>
-  </si>
-  <si>
-    <t>estuary=yes</t>
-  </si>
-  <si>
-    <t>skyscraper|condominium|tall building|high-rise apartment|high-rise building|skyline</t>
-  </si>
-  <si>
-    <t>building=***any*** AND building:levels&gt;10</t>
-  </si>
-  <si>
-    <t>clear cut patch|logging|clear cut area|Logging area|deforested area|strip clearcut</t>
-  </si>
-  <si>
-    <t>landuse=logging, man_made=clearcut, man_made=cutline</t>
-  </si>
-  <si>
-    <t>street lane|Car lane|traffic lane</t>
-  </si>
-  <si>
-    <t>lanes=***numeric***</t>
-  </si>
-  <si>
-    <t>carpool lane|HOV lane|High-occupancy vehicle lane</t>
-  </si>
-  <si>
-    <t>["hov:lanes:forward:conditional"|"hov:lanes:backward:conditional"|"hov:lanes:forward"|"hov:lanes:backward"|"hov:lanes:conditional"|"hov:lanes"]=designated</t>
-  </si>
-  <si>
-    <t>lanes in each direction|lanes going in each direction</t>
-  </si>
-  <si>
-    <t>lanes:forward=***numeric*** AND lanes:backward=***numeric***</t>
-  </si>
-  <si>
-    <t>train station|station|railway station|railway passenger station|railroad station|train platform|train stopping location</t>
-  </si>
-  <si>
-    <t>railway=station, public_transport=station AND train=yes,public_transport=platform AND train=yes, public_transport=stop_position AND train=yes, railway=halt, railway=platform, building=train_station</t>
-  </si>
-  <si>
-    <t>bus stop|bus platform|Bus bay|coach stop area|trolleybus station|trolleybus terminal|trolleybus stopping location</t>
-  </si>
-  <si>
-    <t>highway=bus_stop, bus_bay=both, bus_bay=left, bus_bay=right, public_transport=stop_position AND bus=yes, public_transport=stop_area, public_transport=station AND trolleybus=yes, public_transport=platform AND trolleybus=yes, public_transport=platform AND trolleybus=yes, public_transport=platform AND bus=yes, public_transport=stop_position AND trolleybus=yes, public_transport=platform AND trolleybus=yes</t>
-  </si>
-  <si>
-    <t>bus station|public bus transport station|bus transit station|bus commuter station|bus transport hub|bus interchangeterminus|coach station|</t>
-  </si>
-  <si>
-    <t>public_transport=platform AND bus=yes, public_transport=station AND bus=yes, amenity=bus_station, highway=platform AND bus=yes</t>
-  </si>
-  <si>
-    <t>Tram Stop|Tram Stopping location|Tram Station|Tram Platform</t>
-  </si>
-  <si>
-    <t>public_transport=stop_position AND tram=yes, public_transport=station AND tram=yes, public_transport=platform AND tram=yes, railway=tram_stop</t>
-  </si>
-  <si>
-    <t>subway stop|subway station|subway platform|subway entrance</t>
-  </si>
-  <si>
-    <t>public_transport=platform AND subway=yes, public_transport=stop_position AND subway=yes, public_transport=station AND subway=yes, railway=subway_entrance</t>
-  </si>
-  <si>
-    <t>monorail station|aerialway station|aerialway stopping location|light rail stopping location|monorail stopping location|light rail stop|light rail platform|light rail station|aerialway stop|aerialway platform|monorail platform|monorail stop</t>
-  </si>
-  <si>
-    <t>public_transport=station AND monorail=yes, public_transport=stop_position AND aerialway=yes, public_transport=stop_position AND light_rail=yes, public_transport=stop_position AND monorail=yes, public_transport=station AND light_rail=yes, public_transport=platform AND light_rail=yes, public_transport=platform AND aerialway=yes, public_transport=platform AND subway=yes, public_transport=platform AND monorail=yes</t>
-  </si>
-  <si>
-    <t>Ferry|Ferry terminal|ferry stopping location|ferry platform|ferry dock|public water transit|public water transport|marine terminal| ferry port | ferry arrival | ferry departure</t>
-  </si>
-  <si>
-    <t>amenity=ferry_terminal, public_transport=station AND ferry=yes, public_transport=stop_position AND ferry=yes, public_transport=platform AND ferry=yes</t>
-  </si>
-  <si>
-    <t>spike strip|wicket gate|sally port|stile|bump gate|wire gate|kissing gate|mororcycle barrier|railing|noise barrier|drive through gate</t>
-  </si>
-  <si>
-    <t>barrier=yes, barrier=fence AND fence_type=railing, barrier=wall AND wall=noise_barrier</t>
-  </si>
-  <si>
-    <t>Public Prosecutor's Office|attorney general, district attorney</t>
-  </si>
-  <si>
-    <t>office=government AND government=prosecutor</t>
-  </si>
-  <si>
-    <t>Notary Office</t>
-  </si>
-  <si>
-    <t>office=lawyer AND lawyer=notary</t>
-  </si>
-  <si>
-    <t>Liaison Office|diplomatic mission</t>
-  </si>
-  <si>
-    <t>office=diplomatic AND diplomatic=liaison</t>
-  </si>
-  <si>
-    <t>Consulate|consular post</t>
-  </si>
-  <si>
-    <t>office=diplomatic AND diplomatic=consulate</t>
-  </si>
-  <si>
-    <t>Embassy|foreign mission</t>
-  </si>
-  <si>
-    <t>office=diplomatic AND diplomatic=embassy, amenity=embassy</t>
-  </si>
-  <si>
-    <t>wintersports|sleigh trail|sled run|ski trail|ski touring trail|ice skating trail|ice skating ring|snowshoeing|winter hiking trail|cross-country ski trail|snowsport trail|piste|downhill ski run|snowsports half pipe|snow park|ski jump</t>
-  </si>
-  <si>
-    <t>piste:type=sleigh, piste:type=sled,piste:type=skitour, piste:type=ice_skate, piste:type=hike, piste:type=nordic, piste:type=downhill, piste:type=downhill AND man_made=piste:halfpipe, piste:type=snow_park, piste:type=ski_jump</t>
-  </si>
-  <si>
-    <t>Tourism map|public map|visitor center|public guidepost|trail marker|public information terminal|information terminal|public information board</t>
-  </si>
-  <si>
-    <t>tourism=information AND information=***any***</t>
-  </si>
-  <si>
-    <t>art gallery</t>
-  </si>
-  <si>
-    <t>tourism=gallery</t>
-  </si>
-  <si>
-    <t>public artwork|artwork|bust|statue|sculpture|art installation</t>
-  </si>
-  <si>
-    <t>tourism=artwork, tourism=artwork AND artwork_type=bust, tourism=artwork AND artwork_type=statue, tourism=artwork AND artwork_type=sculpture, tourism=artwork AND artwork_type=installation</t>
-  </si>
-  <si>
-    <t>graffiti|mural</t>
-  </si>
-  <si>
-    <t>tourism=artwork AND artwork_type=graffiti, tourism=artwork AND artwork_type=mural</t>
-  </si>
-  <si>
-    <t>campsite|camping area|camp ground|camping|backpacking site|camp pitch</t>
-  </si>
-  <si>
-    <t>tourism=camp_site, tourism=camp_pitch</t>
-  </si>
-  <si>
-    <t>wetland|Bog|Swamp|String Bog|Coastal Salt Marsh|Fen|reed bed|mangrove|marsh|wet meadow|tidal flat</t>
-  </si>
-  <si>
-    <t>natural=wetland, wetland=***any***</t>
-  </si>
-  <si>
-    <t>Oxbow Lake</t>
-  </si>
-  <si>
-    <t>water=oxbow</t>
-  </si>
-  <si>
-    <t>Dovecote|Dove house|Pigeonhole|Pigeon house|doocot|Dovecot|birdhouse</t>
-  </si>
-  <si>
-    <t>man_made=dovecote</t>
-  </si>
-  <si>
-    <t>Cross|wayside cross</t>
-  </si>
-  <si>
-    <t>man_made=cross, historic=wayside_cross</t>
-  </si>
-  <si>
-    <t>Embankment</t>
-  </si>
-  <si>
-    <t>man_made=embankment</t>
-  </si>
-  <si>
-    <t>Satellite Dish|parabolic dish|satellite communication</t>
-  </si>
-  <si>
-    <t>man_made=satellite_dish</t>
-  </si>
-  <si>
-    <t>Compass Rose|rose of the winds|public compass</t>
-  </si>
-  <si>
-    <t>man_made=compass_rose</t>
-  </si>
-  <si>
-    <t>EV Charging Point|electrical vehicle|electrical charge point| EV charging station|car charging station|charging station</t>
-  </si>
-  <si>
-    <t>man_made=charge_point</t>
-  </si>
-  <si>
-    <t>Flagpole|flag</t>
-  </si>
-  <si>
-    <t>man_made=flagpole</t>
-  </si>
-  <si>
-    <t>Beehive|apiary|beekeeper|honey farm|pollination</t>
-  </si>
-  <si>
-    <t>man_made=beehive</t>
-  </si>
-  <si>
-    <t>Street Cabinet|cable TV cabinet|telecommunications cabinet|technical box|telecom exchange</t>
-  </si>
-  <si>
-    <t>man_made=street_cabinet, telecom=exchange</t>
-  </si>
-  <si>
-    <t>Utility Pole|telephone pole|electricity pole</t>
-  </si>
-  <si>
-    <t>man_made=utility_pole</t>
-  </si>
-  <si>
-    <t>Digital Screen|video wall|public screen|display|led wall</t>
-  </si>
-  <si>
-    <t>man_made=video_wall</t>
-  </si>
-  <si>
-    <t>Tunnel Area|Tunnel|Underground passgae|underpass</t>
-  </si>
-  <si>
-    <t>man_made=tunnel</t>
-  </si>
-  <si>
-    <t>Storage Tank</t>
-  </si>
-  <si>
-    <t>man_made=storage_tank</t>
-  </si>
-  <si>
-    <t>Pagoda|buddhist tower|tiered tower</t>
-  </si>
-  <si>
-    <t>man_made=tower AND tower:type=pagoda</t>
-  </si>
-  <si>
-    <t>Bell Tower|belfry|bell gable|campanile|klockstapel</t>
-  </si>
-  <si>
-    <t>man_made=tower AND tower:type=bell_tower</t>
-  </si>
-  <si>
-    <t>Cosmetics Store|make up shop|make-up shop</t>
-  </si>
-  <si>
-    <t>shop=cosmetics</t>
-  </si>
-  <si>
-    <t>Seafood Shop|fish shop</t>
-  </si>
-  <si>
-    <t>shop=seafood</t>
-  </si>
-  <si>
-    <t>Furniture Store|interior shop</t>
-  </si>
-  <si>
-    <t>shop=furniture</t>
-  </si>
-  <si>
-    <t>Tailor</t>
-  </si>
-  <si>
-    <t>shop=tailor</t>
-  </si>
-  <si>
-    <t>entrance|exit</t>
-  </si>
-  <si>
-    <t>building=entrance</t>
-  </si>
-  <si>
-    <t>Yurt|Ger</t>
-  </si>
-  <si>
-    <t>building=ger</t>
-  </si>
-  <si>
-    <t>Cabin</t>
-  </si>
-  <si>
-    <t>building=cabin</t>
-  </si>
-  <si>
-    <t>Bungalow</t>
-  </si>
-  <si>
-    <t>building=bungalow</t>
-  </si>
-  <si>
-    <t>Allotment House</t>
-  </si>
-  <si>
-    <t>building=allotment_house</t>
-  </si>
-  <si>
-    <t>Boathouse</t>
-  </si>
-  <si>
-    <t>building=boathouse</t>
-  </si>
-  <si>
-    <t>Slaughterhouse|abattoir|butchery|killing house</t>
-  </si>
-  <si>
-    <t>industrial=slaughterhouse</t>
-  </si>
-  <si>
-    <t>Scrap Yard|junk yard|junk shop|scrap heap|wreck yard</t>
-  </si>
-  <si>
-    <t>industrial=scrap_yard</t>
-  </si>
-  <si>
-    <t>Fire Pit|bonfire|campfire|fire place</t>
-  </si>
-  <si>
-    <t>leisure=firepit</t>
-  </si>
-  <si>
-    <t>trampoline park</t>
-  </si>
-  <si>
-    <t>leisure=trampoline_park</t>
-  </si>
-  <si>
-    <t>chess table|public chess board|public chess</t>
-  </si>
-  <si>
-    <t>leisure=picnic_table AND sport=chess, sport=chess</t>
-  </si>
-  <si>
-    <t>resort|sanatorium|vacation resort</t>
-  </si>
-  <si>
-    <t>leisure=resort</t>
-  </si>
-  <si>
-    <t>public fitness|public exercise|outdoor fitness|outdoor exercise</t>
-  </si>
-  <si>
-    <t>leisure=fitness_station</t>
-  </si>
-  <si>
-    <t>padel court|padel</t>
-  </si>
-  <si>
-    <t>sport=padel</t>
-  </si>
-  <si>
-    <t>boules|bocce court|pétanque|pétangue|petanque|bocce|jeu de boules</t>
-  </si>
-  <si>
-    <t>sport=boules</t>
-  </si>
-  <si>
-    <t>skate park|bmx|skateboarding|skatepark</t>
-  </si>
-  <si>
-    <t>sport=skateboard</t>
-  </si>
-  <si>
-    <t>rugby league field|rugby union field|rugby field</t>
-  </si>
-  <si>
-    <t>sport=rugby_league, sport=rugby_union</t>
-  </si>
-  <si>
-    <t>australian football field|AFL</t>
-  </si>
-  <si>
-    <t>sport=australian_football</t>
-  </si>
-  <si>
-    <t>bowling green</t>
-  </si>
-  <si>
-    <t>sport=bowls</t>
-  </si>
-  <si>
-    <t>four square court|4square|4 square</t>
-  </si>
-  <si>
-    <t>sport=four_square</t>
-  </si>
-  <si>
-    <t>ping pong table|table tennis</t>
-  </si>
-  <si>
-    <t>sport=table_tennis</t>
-  </si>
-  <si>
-    <t>cricket field|cricket</t>
-  </si>
-  <si>
-    <t>sport=cricket</t>
-  </si>
-  <si>
-    <t>team handball court|handball</t>
-  </si>
-  <si>
-    <t>sport=handball, sport=american_handball</t>
-  </si>
-  <si>
-    <t>beach volleyball court|beach volleyball</t>
-  </si>
-  <si>
-    <t>sport=beachvolleyball</t>
-  </si>
-  <si>
-    <t>shooting Range|firing range|gun range|shooting gallery|gun practice|shooting practice|target practice</t>
-  </si>
-  <si>
-    <t>sport=shooting</t>
-  </si>
-  <si>
-    <t>hammer throw ring|hammer throw</t>
-  </si>
-  <si>
-    <t>sport=athletics AND athletics=hammer_throw</t>
-  </si>
-  <si>
-    <t>shot put ring|shot put pit</t>
-  </si>
-  <si>
-    <t>sport=athletics AND athletics=shot_put</t>
-  </si>
-  <si>
-    <t>paintball field</t>
-  </si>
-  <si>
-    <t>sport=paintball</t>
-  </si>
-  <si>
-    <t>funnel ball court</t>
-  </si>
-  <si>
-    <t>sport=funnel_ball</t>
-  </si>
-  <si>
-    <t>softball field</t>
-  </si>
-  <si>
-    <t>sport=softball</t>
-  </si>
-  <si>
-    <t>american football field</t>
-  </si>
-  <si>
-    <t>sport=american_football</t>
-  </si>
-  <si>
-    <t>archery range|bow and arrow|crossbow|bow shooting</t>
-  </si>
-  <si>
-    <t>sport=archery</t>
-  </si>
-  <si>
-    <t>netball</t>
-  </si>
-  <si>
-    <t>sport=netball</t>
-  </si>
-  <si>
-    <t>tetherball|swingball</t>
-  </si>
-  <si>
-    <t>sport=tetherball</t>
-  </si>
-  <si>
-    <t>field hockey</t>
-  </si>
-  <si>
-    <t>sport=field_hockey</t>
-  </si>
-  <si>
-    <t>shuffleboard</t>
-  </si>
-  <si>
-    <t>sport=shuffleboard</t>
-  </si>
-  <si>
-    <t>gaga pit</t>
-  </si>
-  <si>
-    <t>sport=gaga</t>
-  </si>
-  <si>
-    <t>badminton</t>
-  </si>
-  <si>
-    <t>sport=badminton</t>
-  </si>
-  <si>
-    <t>volleyball</t>
-  </si>
-  <si>
-    <t>sport=volleyball</t>
-  </si>
-  <si>
-    <t>pickleball court</t>
-  </si>
-  <si>
-    <t>sport=pickleball</t>
-  </si>
-  <si>
-    <t>yoga|yoga studio|asanas|meditation center|meditation studio</t>
-  </si>
-  <si>
-    <t>sport=yoga</t>
-  </si>
-  <si>
-    <t>climbing gym|climbing center|boulder center|bouldering|rock climbing|rock gym|climbing wall|boulder gym</t>
-  </si>
-  <si>
-    <t>sport=climbing, climbing=boulder, climbing:boulder=yes</t>
-  </si>
-  <si>
-    <t>adventure park|obstacle course|rope climbing</t>
-  </si>
-  <si>
-    <t>sport=climbing_adventure</t>
-  </si>
-  <si>
-    <t>community garden|co-op garden|collective garden|communal garden</t>
-  </si>
-  <si>
-    <t>leisure=garden AND garden:type=community</t>
-  </si>
-  <si>
-    <t>botanical garden|rare plants|botanic garden</t>
-  </si>
-  <si>
-    <t>leisure=garden AND garden:type=botanical</t>
-  </si>
-  <si>
-    <t>residential garden|back garden|back yard|domestic garden|front garden|front yard|private garden</t>
-  </si>
-  <si>
-    <t>leisure=garden AND garden:type=residential</t>
-  </si>
-  <si>
-    <t>traffic calming|speed bump|speed hump|speed table|traffic island|speed cushion|traffic choker|traffic rumble strip|chicane|traffic chicane</t>
-  </si>
-  <si>
-    <t>traffic_calming=***any***</t>
-  </si>
-  <si>
-    <t>smoking area|smokers' area</t>
-  </si>
-  <si>
-    <t>amenity=smoking_area</t>
-  </si>
-  <si>
-    <t>dojo|martial arts|dojang</t>
-  </si>
-  <si>
-    <t>amenity=dojo</t>
-  </si>
-  <si>
-    <t>coworking space|coworking place|coworking office</t>
-  </si>
-  <si>
-    <t>amenity=coworking_space</t>
-  </si>
-  <si>
-    <t>permanent polling place|ballot box|ballot drop|polling place|voting booth|voting machine|polling station</t>
-  </si>
-  <si>
-    <t>amenity=polling_station</t>
-  </si>
-  <si>
-    <t>shisha lounge|hookah lounge|waterpipe|nargile</t>
-  </si>
-  <si>
-    <t>amenity=hookah_lounge</t>
-  </si>
-  <si>
-    <t>second hand shop|2nd hand shop</t>
-  </si>
-  <si>
-    <t>amenity=recycling AND recycling:electrical_items=yes</t>
-  </si>
-  <si>
-    <t>green waste|biodegradable waste|biological waste|compost</t>
-  </si>
-  <si>
-    <t>amenity=recycling AND recycling:green_waste=yes</t>
-  </si>
-  <si>
-    <t>abortion clinic</t>
-  </si>
-  <si>
-    <t>healthcare:speciality=abortion</t>
-  </si>
-  <si>
-    <t>transit shelter|public transport shelter</t>
-  </si>
-  <si>
-    <t>amenity=shelter AND shelter_type=public_transport</t>
-  </si>
-  <si>
-    <t>nightclub|dance club|dancing|disco|discotheque|night club</t>
-  </si>
-  <si>
-    <t>amenity=nightclub</t>
-  </si>
-  <si>
-    <t>place of worship|house of god|house of worship</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship, building=cathedral, building=chapel, building=church, building=mosque, building=shrine, building=synagogue, building=temple</t>
-  </si>
-  <si>
-    <t>religion</t>
-  </si>
-  <si>
-    <t>religion=***example***</t>
-  </si>
-  <si>
-    <t>denomination</t>
-  </si>
-  <si>
-    <t>denomination=***example***</t>
-  </si>
-  <si>
-    <t>Sikh Temple</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=sikh</t>
-  </si>
-  <si>
-    <t>Shinto Shrine</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=shinto</t>
-  </si>
-  <si>
-    <t>Jewish Synagogue|synagogue|shul|jewish temple|jewish house of worship</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=jewish, building=synagogue</t>
-  </si>
-  <si>
-    <t>Taoist Temple</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=taoist</t>
-  </si>
-  <si>
-    <t>Christian Church</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship  AND religion=christian</t>
-  </si>
-  <si>
-    <t>Muslim Mosque</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=muslim, building=mosque</t>
-  </si>
-  <si>
-    <t>Minaret|Muezzin</t>
-  </si>
-  <si>
-    <t>man_made=tower AND tower:type=minaret</t>
-  </si>
-  <si>
-    <t>Buddhist Temple</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship  AND religion=buddhist</t>
-  </si>
-  <si>
-    <t>Hindu Temple</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=hindu</t>
-  </si>
-  <si>
-    <t>Kingdom Hall of Jehovah's Witnesses</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=christian AND denomination=jehovahs_witness</t>
-  </si>
-  <si>
-    <t>La Luz del Mundo Temple</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=christian AND denomination=la_luz_del_mundo</t>
-  </si>
-  <si>
-    <t>Quaker Friends Meeting House</t>
-  </si>
-  <si>
-    <t>amenity=place_of_worship AND religion=christian AND denomination=quaker</t>
-  </si>
-  <si>
-    <t>manhole</t>
-  </si>
-  <si>
-    <t>manhole=***any***</t>
-  </si>
-  <si>
-    <t>lighting mast|flood light|stadium lights|stadium lighting</t>
-  </si>
-  <si>
-    <t>man_made=mast AND tower:type=lighting</t>
-  </si>
-  <si>
-    <t>water tank|cistern|water tower</t>
-  </si>
-  <si>
-    <t>man_made=storage_tank AND content=water, man_made=water_tower, building=water_tower, emergency=water_tank</t>
-  </si>
-  <si>
-    <t>communication mast|broadcast tower|communication antenna|cell phone tower|mobile phone mast|radio broadcast mast|radio tower|transmission tower|tv mast|tv tower|communication tower|cell tower</t>
-  </si>
-  <si>
-    <t>man_made=communications_tower, man_made=mast AND tower:type=communication, man_made=tower AND tower:type=communication</t>
-  </si>
-  <si>
-    <t>radio telescope|ground station|radio dish|radio antenna</t>
-  </si>
-  <si>
-    <t>man_made=telescope, telescope:type=radio</t>
-  </si>
-  <si>
-    <t>optical telescope|refracting telescope|reflecting telescope</t>
-  </si>
-  <si>
-    <t>man_made=telescope, telescope:type=optical</t>
-  </si>
-  <si>
-    <t>crane|gantry crane|portal crane|overhead crane|gantry</t>
-  </si>
-  <si>
-    <t>man_made=crane AND crane:type=***any***, man_made=gantry</t>
-  </si>
-  <si>
-    <t>postal relay box|post relay box</t>
-  </si>
-  <si>
-    <t>man_made=street_cabinet AND street_cabinet=postal_service</t>
-  </si>
-  <si>
-    <t>traffic monitoring cabinet|traffic count|traffic count box|vehicle counting</t>
-  </si>
-  <si>
-    <t>man_made=street_cabinet AND street_cabinet=traffic_monitoring</t>
-  </si>
-  <si>
-    <t>first aid kit|med kit|medkit</t>
-  </si>
-  <si>
-    <t>emergency=first_aid_kit</t>
-  </si>
-  <si>
-    <t>lifeboat|marine rescue|boat rescue|lifeboat station</t>
-  </si>
-  <si>
-    <t>emergency=water_rescue</t>
-  </si>
-  <si>
-    <t>Wi-Fi Hotspot|wi-fi|public wifi|hotspot</t>
-  </si>
-  <si>
-    <t>internet_access=wlan</t>
-  </si>
-  <si>
-    <t>Antenna</t>
-  </si>
-  <si>
-    <t>man_made=antenna</t>
-  </si>
-  <si>
-    <t>Courtyard|yard</t>
-  </si>
-  <si>
-    <t>man_made=courtyard</t>
-  </si>
-  <si>
-    <t>Torii|japanese gate|Shinto gate</t>
-  </si>
-  <si>
-    <t>man_made=torii</t>
-  </si>
-  <si>
-    <t>Obelisk</t>
-  </si>
-  <si>
-    <t>man_made=obelisk</t>
-  </si>
-  <si>
-    <t>Water Works</t>
-  </si>
-  <si>
-    <t>man_made=water_works</t>
-  </si>
-  <si>
-    <t>Beacon</t>
-  </si>
-  <si>
-    <t>man_made=beacon</t>
-  </si>
-  <si>
-    <t>Wind Turbine|aerorotor</t>
-  </si>
-  <si>
-    <t>power=generator AND generator:source=wind, generator:method=wind_turbine, plant:method=wind_turbine, generator:type=wind_turbine</t>
-  </si>
-  <si>
-    <t>windmill|wind pump</t>
-  </si>
-  <si>
-    <t>man_made=windmill, man_made=windpump</t>
-  </si>
-  <si>
-    <t>Nuclear Reactor</t>
-  </si>
-  <si>
-    <t>power=generator AND generator:source=nuclear, power=generator AND generator:method=fission</t>
-  </si>
-  <si>
-    <t>Water Turbine|water dam|hydroelectricity</t>
-  </si>
-  <si>
-    <t>power=generator AND generator:source=hydro</t>
-  </si>
-  <si>
-    <t>Solar Panel|photovoltaic|PV|sunlight energy|solar power plant|solar energy plant</t>
-  </si>
-  <si>
-    <t>power=generator AND generator:method=photovoltaic, power=plant AND plant:source=solar</t>
-  </si>
-  <si>
-    <t>Wind Farm|offshore wind|wind park|wind power plant|wind energy plant</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=wind</t>
-  </si>
-  <si>
-    <t>Waste Incineration Power Plant|garbage incinerator</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=waste</t>
-  </si>
-  <si>
-    <t>Coal-Fired Power Plant|coal fired energy plant</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=coal</t>
-  </si>
-  <si>
-    <t>Nuclear Power Plant|atomic power plant|nuclear energy plant</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=nuclear</t>
-  </si>
-  <si>
-    <t>Cooling Tower</t>
-  </si>
-  <si>
-    <t>man_made=tower AND tower:type=cooling</t>
-  </si>
-  <si>
-    <t>Hydroelectric Power Station|water power plant|tidal power plant|hydro power plant</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=hydro</t>
-  </si>
-  <si>
-    <t>Oil-Fired Power Plant|oil power station</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=oil</t>
-  </si>
-  <si>
-    <t>Gas-Fired Power Plant|gas power station</t>
-  </si>
-  <si>
-    <t>power=plant AND plant:source=gas</t>
-  </si>
-  <si>
-    <t>Parking Ticket Vending Machine|parking ticket</t>
-  </si>
-  <si>
-    <t>amenity=vending_machine AND vending=parking_tickets</t>
-  </si>
-  <si>
-    <t>Cycling track|running track|athletics track</t>
-  </si>
-  <si>
-    <t>leisure=track AND sport=cycling, leisure=track AND sport=running, leisure=track AND sport=athletics, sport=athletics</t>
-  </si>
-  <si>
-    <t>Horse Racetrack|equestrian race track|horse racing</t>
-  </si>
-  <si>
-    <t>sport=horse_racing</t>
-  </si>
-  <si>
-    <t>Advertising Totem|Poster Box|Billboard|Notice Board|advertising board|advertising column|advertising screen|advertising sign|advertising tarp|wall painting</t>
-  </si>
-  <si>
-    <t>advertising=***any***</t>
-  </si>
-  <si>
-    <t>Destination Sign</t>
-  </si>
-  <si>
-    <t>street_sign=destination_sign</t>
-  </si>
-  <si>
-    <t>Hiking route|walking route|outdoor sports|bicycle route</t>
-  </si>
-  <si>
-    <t>route=hiking, route=bicyle, route=walking</t>
-  </si>
-  <si>
-    <t>public transport routes | bus route | tram route |metro route</t>
-  </si>
-  <si>
-    <t>route=bus, route= train, route= ferry, route=tram, route= trolleybus, route=subway</t>
-  </si>
-  <si>
-    <t>Garden Center|flower store</t>
-  </si>
-  <si>
-    <t>shop=garden_centre, shop=flowers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer Store </t>
-  </si>
-  <si>
-    <t>shop=computer</t>
-  </si>
-  <si>
-    <t>rental shop</t>
-  </si>
-  <si>
-    <t>shop=rental</t>
-  </si>
-  <si>
-    <t>Chocolate Store|candy store</t>
-  </si>
-  <si>
-    <t>Outdoor store</t>
-  </si>
-  <si>
-    <t>shop=outdoor</t>
-  </si>
-  <si>
-    <t>Funeral Home|morgue|crematorium|mortuary</t>
-  </si>
-  <si>
-    <t>shop=funeral_directors, amenity=mortuary</t>
-  </si>
-  <si>
-    <t>Storage Rental</t>
-  </si>
-  <si>
-    <t>shop=storage_rental</t>
-  </si>
-  <si>
-    <t>Erotic Store | sex shop</t>
-  </si>
-  <si>
-    <t>shop=erotic, shop=sex</t>
-  </si>
-  <si>
-    <t>Motorcycle Repair Shop</t>
-  </si>
-  <si>
-    <t>shop=motorcycle_repair</t>
-  </si>
-  <si>
-    <t>Butcher</t>
-  </si>
-  <si>
-    <t>shop=butcher</t>
-  </si>
-  <si>
-    <t>Arts &amp; Crafts Store</t>
-  </si>
-  <si>
-    <t>shop=craft</t>
-  </si>
-  <si>
-    <t>Furnishing Store|carpet|curtains|mattress|luggage</t>
-  </si>
-  <si>
-    <t>shop=bathroom_furnishing, shop=carpet, shop=curtains, shop=bed, shop=luggage</t>
-  </si>
-  <si>
-    <t>house number|building number</t>
-  </si>
-  <si>
-    <t>addr:housenumber=***example***</t>
-  </si>
-  <si>
-    <t>roof material</t>
-  </si>
-  <si>
-    <t>roof:material=***example***</t>
-  </si>
-  <si>
-    <t>elevator</t>
-  </si>
-  <si>
-    <t>elevator=yes</t>
-  </si>
-  <si>
-    <t>pet shop|animal shop</t>
-  </si>
-  <si>
-    <t>shop=pet, shop=pet_grooming</t>
-  </si>
-  <si>
-    <t>stadium|stadion|pitch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leisure=stadium, leisure=pitch, building=stadium, stadium=football, stadium=soccer, </t>
-  </si>
-  <si>
-    <t>sport</t>
-  </si>
-  <si>
-    <t>sport=***example***</t>
-  </si>
-  <si>
-    <t>school|highschool|elementary school|school building|language school|music school|learning center|preparatory school|prep school</t>
-  </si>
-  <si>
-    <t>car rental|car sharing parking lot|Car sharing spots|car sharing place|hire car|car pool|car pooling station</t>
-  </si>
-  <si>
-    <t>parking spaces|parking spots|parking|parking area|Parking lots|parking zone|parking aisle|street side parking| parking space|parking spot| parking slot| parking place| parking stall|accessible parking space</t>
-  </si>
-  <si>
-    <t>community centre|rec center|recreation center|community hall|activity center|neighborhood center|cultural center|civic centre</t>
-  </si>
-  <si>
-    <t>amenity=community_centre, amenity=social_centre</t>
-  </si>
-  <si>
-    <t>conference centre|convention center|meeting venue|conference facility|symposium center|exhibition center|trade fair|trade fair center|congress center</t>
-  </si>
-  <si>
-    <t>TV studio|radio studio|recording studio|production studio|sound studio|music studio|audio lab|broadcasting studio|news studio|film studio</t>
-  </si>
-  <si>
-    <t>amenity=toilets, building=toilets, toilets=yes</t>
-  </si>
-  <si>
-    <t>refugee site| refugee camp| refugee center| refugee settlement| refugee shelter| displaced persons camp</t>
-  </si>
-  <si>
-    <t>amenity=refugee_site</t>
-  </si>
-  <si>
-    <t>service</t>
-  </si>
-  <si>
-    <t>fire tower|observation tower|lookout tower</t>
-  </si>
-  <si>
-    <t>man_made=tower AND tower:type=observation</t>
-  </si>
-  <si>
-    <t>lifeguard spot</t>
-  </si>
-  <si>
-    <t>speed camera</t>
-  </si>
-  <si>
-    <t>highway=street_lamp</t>
-  </si>
-  <si>
-    <t>Military Trench|war trench</t>
-  </si>
-  <si>
-    <t>winter sports</t>
-  </si>
-  <si>
-    <t>stadium|stadium building</t>
-  </si>
-  <si>
-    <t>leisure=stadium, building=stadium</t>
-  </si>
-  <si>
-    <t>estate agent</t>
-  </si>
-  <si>
-    <t>politician's office</t>
-  </si>
-  <si>
-    <t>office of a political party</t>
   </si>
   <si>
     <t>supermarket|discount|wholesale</t>
@@ -4160,8 +4169,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Gut" xfId="1" builtinId="26"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4510,11 +4519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E391F786-B0DC-574F-BA27-B454063FA60E}">
-  <dimension ref="A1:H605"/>
+  <dimension ref="A1:H606"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <pane ySplit="1" topLeftCell="B591" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F607" sqref="F607"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -13427,6 +13436,17 @@
       </c>
       <c r="F605" s="2" t="s">
         <v>1225</v>
+      </c>
+    </row>
+    <row r="606" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B606" s="2" t="s">
+        <v>1226</v>
+      </c>
+      <c r="D606" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F606" s="2" t="s">
+        <v>1227</v>
       </c>
     </row>
   </sheetData>
@@ -13737,7 +13757,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>14</v>
@@ -13834,7 +13854,7 @@
         <v>53</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>8</v>
@@ -13919,7 +13939,7 @@
         <v>64</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
@@ -14194,7 +14214,7 @@
         <v>84</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>2</v>
@@ -14203,7 +14223,7 @@
         <v>9</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.95">
@@ -14222,7 +14242,7 @@
         <v>85</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>2</v>
@@ -14307,7 +14327,7 @@
         <v>97</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>8</v>
@@ -14554,7 +14574,7 @@
         <v>3</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="15.95">
@@ -14786,7 +14806,7 @@
         <v>151</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>14</v>
@@ -14795,7 +14815,7 @@
         <v>9</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="15.95">
@@ -15620,7 +15640,7 @@
         <v>283</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="D133" s="6" t="s">
         <v>3</v>
@@ -15968,13 +15988,13 @@
     </row>
     <row r="157" spans="1:6" ht="15.95">
       <c r="B157" s="2" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="D157" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="158" spans="1:6" ht="15.95">
@@ -15996,7 +16016,7 @@
         <v>410</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="D159" s="6" t="s">
         <v>9</v>
@@ -16574,7 +16594,7 @@
         <v>542</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="D196" s="6" t="s">
         <v>9</v>
@@ -16630,7 +16650,7 @@
         <v>9</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="15.95">
@@ -17090,7 +17110,7 @@
     </row>
     <row r="229" spans="1:6" ht="15.95">
       <c r="B229" s="2" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>9</v>
@@ -17155,7 +17175,7 @@
         <v>636</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>14</v>
@@ -17398,7 +17418,7 @@
         <v>665</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>14</v>
@@ -17407,7 +17427,7 @@
         <v>3</v>
       </c>
       <c r="F248" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="249" spans="1:6" ht="15.95">
@@ -18347,7 +18367,7 @@
         <v>807</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="D310" s="6" t="s">
         <v>3</v>
@@ -18487,7 +18507,7 @@
         <v>825</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
       <c r="D320" s="6" t="s">
         <v>3</v>
@@ -18501,7 +18521,7 @@
         <v>826</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="D321" s="6" t="s">
         <v>3</v>
@@ -18710,7 +18730,7 @@
         <v>892</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>681</v>
+        <v>1251</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>14</v>
@@ -18975,7 +18995,7 @@
         <v>1000</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>1249</v>
+        <v>1252</v>
       </c>
       <c r="C351" s="2" t="s">
         <v>2</v>
@@ -19286,7 +19306,7 @@
         <v>1092</v>
       </c>
       <c r="B373" s="2" t="s">
-        <v>1250</v>
+        <v>1253</v>
       </c>
       <c r="D373" s="6" t="s">
         <v>9</v>
@@ -19300,7 +19320,7 @@
         <v>1096</v>
       </c>
       <c r="B374" s="2" t="s">
-        <v>1251</v>
+        <v>1254</v>
       </c>
       <c r="D374" s="6" t="s">
         <v>9</v>
@@ -19747,7 +19767,7 @@
         <v>9</v>
       </c>
       <c r="F404" s="2" t="s">
-        <v>1252</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="405" spans="1:6" ht="15.95">
@@ -19764,7 +19784,7 @@
         <v>3</v>
       </c>
       <c r="F405" s="2" t="s">
-        <v>1253</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="406" spans="1:6" ht="15.95">
@@ -19851,7 +19871,7 @@
         <v>1296</v>
       </c>
       <c r="B411" s="2" t="s">
-        <v>1254</v>
+        <v>1257</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>14</v>
@@ -20197,7 +20217,7 @@
         <v>9005</v>
       </c>
       <c r="B434" s="2" t="s">
-        <v>1255</v>
+        <v>1258</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>14</v>
@@ -20606,7 +20626,7 @@
     </row>
     <row r="466" spans="2:6" ht="15.95">
       <c r="B466" s="2" t="s">
-        <v>1256</v>
+        <v>1259</v>
       </c>
       <c r="D466" s="6" t="s">
         <v>9</v>
@@ -20865,7 +20885,7 @@
     </row>
     <row r="489" spans="2:6" ht="15.95">
       <c r="B489" s="2" t="s">
-        <v>1257</v>
+        <v>1260</v>
       </c>
       <c r="C489" s="2" t="s">
         <v>14</v>
@@ -20879,7 +20899,7 @@
     </row>
     <row r="490" spans="2:6" ht="15.95">
       <c r="B490" s="2" t="s">
-        <v>1258</v>
+        <v>1261</v>
       </c>
       <c r="D490" s="6" t="s">
         <v>3</v>
@@ -20890,7 +20910,7 @@
     </row>
     <row r="491" spans="2:6" ht="15.95">
       <c r="B491" s="2" t="s">
-        <v>1259</v>
+        <v>1262</v>
       </c>
       <c r="C491" s="2" t="s">
         <v>14</v>
@@ -20918,7 +20938,7 @@
     </row>
     <row r="493" spans="2:6" ht="15.95">
       <c r="B493" s="2" t="s">
-        <v>1260</v>
+        <v>1263</v>
       </c>
       <c r="C493" s="2" t="s">
         <v>14</v>
@@ -20932,7 +20952,7 @@
     </row>
     <row r="494" spans="2:6" ht="15.95">
       <c r="B494" s="2" t="s">
-        <v>1261</v>
+        <v>1264</v>
       </c>
       <c r="C494" s="2" t="s">
         <v>14</v>
@@ -20946,7 +20966,7 @@
     </row>
     <row r="495" spans="2:6" ht="15.95">
       <c r="B495" s="2" t="s">
-        <v>1262</v>
+        <v>1265</v>
       </c>
       <c r="C495" s="2" t="s">
         <v>14</v>
@@ -20960,7 +20980,7 @@
     </row>
     <row r="496" spans="2:6" ht="15.95">
       <c r="B496" s="2" t="s">
-        <v>1263</v>
+        <v>1266</v>
       </c>
       <c r="C496" s="2" t="s">
         <v>14</v>
@@ -20974,7 +20994,7 @@
     </row>
     <row r="497" spans="2:6" ht="15.95">
       <c r="B497" s="2" t="s">
-        <v>1264</v>
+        <v>1267</v>
       </c>
       <c r="C497" s="2" t="s">
         <v>14</v>
@@ -20988,7 +21008,7 @@
     </row>
     <row r="498" spans="2:6" ht="15.95">
       <c r="B498" s="2" t="s">
-        <v>1265</v>
+        <v>1268</v>
       </c>
       <c r="C498" s="2" t="s">
         <v>14</v>
@@ -21002,7 +21022,7 @@
     </row>
     <row r="499" spans="2:6" ht="15.95">
       <c r="B499" s="2" t="s">
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="C499" s="2" t="s">
         <v>14</v>
@@ -21016,7 +21036,7 @@
     </row>
     <row r="500" spans="2:6" ht="15.95">
       <c r="B500" s="2" t="s">
-        <v>1267</v>
+        <v>1270</v>
       </c>
       <c r="C500" s="2" t="s">
         <v>14</v>
@@ -21030,7 +21050,7 @@
     </row>
     <row r="501" spans="2:6" ht="15.95">
       <c r="B501" s="2" t="s">
-        <v>1268</v>
+        <v>1271</v>
       </c>
       <c r="C501" s="2" t="s">
         <v>14</v>
@@ -21044,7 +21064,7 @@
     </row>
     <row r="502" spans="2:6" ht="15.95">
       <c r="B502" s="2" t="s">
-        <v>1269</v>
+        <v>1272</v>
       </c>
       <c r="C502" s="2" t="s">
         <v>14</v>
@@ -21058,7 +21078,7 @@
     </row>
     <row r="503" spans="2:6" ht="15.95">
       <c r="B503" s="2" t="s">
-        <v>1270</v>
+        <v>1273</v>
       </c>
       <c r="C503" s="2" t="s">
         <v>14</v>
@@ -21072,7 +21092,7 @@
     </row>
     <row r="504" spans="2:6" ht="15.95">
       <c r="B504" s="2" t="s">
-        <v>1271</v>
+        <v>1274</v>
       </c>
       <c r="C504" s="2" t="s">
         <v>14</v>
@@ -21086,7 +21106,7 @@
     </row>
     <row r="505" spans="2:6" ht="15.95">
       <c r="B505" s="2" t="s">
-        <v>1272</v>
+        <v>1275</v>
       </c>
       <c r="C505" s="2" t="s">
         <v>14</v>
@@ -21100,7 +21120,7 @@
     </row>
     <row r="506" spans="2:6" ht="15.95">
       <c r="B506" s="2" t="s">
-        <v>1273</v>
+        <v>1276</v>
       </c>
       <c r="C506" s="2" t="s">
         <v>14</v>
@@ -21114,7 +21134,7 @@
     </row>
     <row r="507" spans="2:6" ht="15.95">
       <c r="B507" s="2" t="s">
-        <v>1274</v>
+        <v>1277</v>
       </c>
       <c r="C507" s="2" t="s">
         <v>14</v>
@@ -21128,7 +21148,7 @@
     </row>
     <row r="508" spans="2:6" ht="15.95">
       <c r="B508" s="2" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="C508" s="2" t="s">
         <v>14</v>
@@ -21142,7 +21162,7 @@
     </row>
     <row r="509" spans="2:6" ht="15.95">
       <c r="B509" s="2" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="C509" s="2" t="s">
         <v>14</v>
@@ -21156,7 +21176,7 @@
     </row>
     <row r="510" spans="2:6" ht="15.95">
       <c r="B510" s="2" t="s">
-        <v>1277</v>
+        <v>1280</v>
       </c>
       <c r="C510" s="2" t="s">
         <v>14</v>
@@ -21170,7 +21190,7 @@
     </row>
     <row r="511" spans="2:6" ht="15.95">
       <c r="B511" s="2" t="s">
-        <v>1278</v>
+        <v>1281</v>
       </c>
       <c r="C511" s="2" t="s">
         <v>14</v>
@@ -21184,7 +21204,7 @@
     </row>
     <row r="512" spans="2:6" ht="15.95">
       <c r="B512" s="2" t="s">
-        <v>1279</v>
+        <v>1282</v>
       </c>
       <c r="C512" s="2" t="s">
         <v>14</v>
@@ -21198,7 +21218,7 @@
     </row>
     <row r="513" spans="2:6" ht="15.95">
       <c r="B513" s="2" t="s">
-        <v>1280</v>
+        <v>1283</v>
       </c>
       <c r="C513" s="2" t="s">
         <v>14</v>
@@ -21212,7 +21232,7 @@
     </row>
     <row r="514" spans="2:6" ht="15.95">
       <c r="B514" s="2" t="s">
-        <v>1281</v>
+        <v>1284</v>
       </c>
       <c r="C514" s="2" t="s">
         <v>14</v>
@@ -21226,7 +21246,7 @@
     </row>
     <row r="515" spans="2:6" ht="15.95">
       <c r="B515" s="2" t="s">
-        <v>1282</v>
+        <v>1285</v>
       </c>
       <c r="C515" s="2" t="s">
         <v>14</v>
@@ -21240,7 +21260,7 @@
     </row>
     <row r="516" spans="2:6" ht="15.95">
       <c r="B516" s="2" t="s">
-        <v>1283</v>
+        <v>1286</v>
       </c>
       <c r="C516" s="2" t="s">
         <v>14</v>
@@ -21254,7 +21274,7 @@
     </row>
     <row r="517" spans="2:6" ht="15.95">
       <c r="B517" s="2" t="s">
-        <v>1284</v>
+        <v>1287</v>
       </c>
       <c r="C517" s="2" t="s">
         <v>14</v>
@@ -21268,7 +21288,7 @@
     </row>
     <row r="518" spans="2:6" ht="15.95">
       <c r="B518" s="2" t="s">
-        <v>1285</v>
+        <v>1288</v>
       </c>
       <c r="C518" s="2" t="s">
         <v>14</v>
@@ -21282,7 +21302,7 @@
     </row>
     <row r="519" spans="2:6" ht="15.95">
       <c r="B519" s="2" t="s">
-        <v>1286</v>
+        <v>1289</v>
       </c>
       <c r="C519" s="2" t="s">
         <v>14</v>
@@ -21296,7 +21316,7 @@
     </row>
     <row r="520" spans="2:6" ht="15.95">
       <c r="B520" s="2" t="s">
-        <v>1287</v>
+        <v>1290</v>
       </c>
       <c r="D520" s="6" t="s">
         <v>9</v>
@@ -21332,7 +21352,7 @@
     </row>
     <row r="523" spans="2:6" ht="15.95">
       <c r="B523" s="2" t="s">
-        <v>1288</v>
+        <v>1291</v>
       </c>
       <c r="C523" s="2" t="s">
         <v>14</v>
@@ -21346,7 +21366,7 @@
     </row>
     <row r="524" spans="2:6" ht="15.95">
       <c r="B524" s="2" t="s">
-        <v>1289</v>
+        <v>1292</v>
       </c>
       <c r="C524" s="2" t="s">
         <v>14</v>
@@ -21360,7 +21380,7 @@
     </row>
     <row r="525" spans="2:6" ht="15.95">
       <c r="B525" s="2" t="s">
-        <v>1290</v>
+        <v>1293</v>
       </c>
       <c r="C525" s="2" t="s">
         <v>14</v>
@@ -21399,7 +21419,7 @@
     </row>
     <row r="528" spans="2:6" ht="15.95">
       <c r="B528" s="2" t="s">
-        <v>1291</v>
+        <v>1294</v>
       </c>
       <c r="D528" s="6" t="s">
         <v>9</v>
@@ -21410,7 +21430,7 @@
     </row>
     <row r="529" spans="1:6" ht="15.95">
       <c r="B529" s="2" t="s">
-        <v>1292</v>
+        <v>1295</v>
       </c>
       <c r="D529" s="6" t="s">
         <v>9</v>
@@ -21421,7 +21441,7 @@
     </row>
     <row r="530" spans="1:6" ht="15.95">
       <c r="B530" s="2" t="s">
-        <v>1293</v>
+        <v>1296</v>
       </c>
       <c r="D530" s="6" t="s">
         <v>9</v>
@@ -21432,7 +21452,7 @@
     </row>
     <row r="531" spans="1:6" ht="15.95">
       <c r="B531" s="2" t="s">
-        <v>1294</v>
+        <v>1297</v>
       </c>
       <c r="D531" s="6" t="s">
         <v>9</v>
@@ -21443,7 +21463,7 @@
     </row>
     <row r="532" spans="1:6" ht="15.95">
       <c r="B532" s="2" t="s">
-        <v>1295</v>
+        <v>1298</v>
       </c>
       <c r="D532" s="6" t="s">
         <v>3</v>
@@ -21454,7 +21474,7 @@
     </row>
     <row r="533" spans="1:6" ht="15.95">
       <c r="B533" s="2" t="s">
-        <v>1296</v>
+        <v>1299</v>
       </c>
       <c r="D533" s="6" t="s">
         <v>3</v>
@@ -21465,7 +21485,7 @@
     </row>
     <row r="534" spans="1:6" ht="15.95">
       <c r="B534" s="2" t="s">
-        <v>1297</v>
+        <v>1300</v>
       </c>
       <c r="C534" s="2" t="s">
         <v>14</v>
@@ -21479,7 +21499,7 @@
     </row>
     <row r="535" spans="1:6" ht="15.95">
       <c r="B535" s="2" t="s">
-        <v>1298</v>
+        <v>1301</v>
       </c>
       <c r="D535" s="6" t="s">
         <v>3</v>
@@ -21755,7 +21775,7 @@
     </row>
     <row r="553" spans="1:6" ht="15.75" customHeight="1">
       <c r="B553" s="2" t="s">
-        <v>1299</v>
+        <v>1302</v>
       </c>
       <c r="D553" s="6" t="s">
         <v>9</v>
@@ -21766,7 +21786,7 @@
     </row>
     <row r="554" spans="1:6" ht="15.75" customHeight="1">
       <c r="B554" s="2" t="s">
-        <v>1300</v>
+        <v>1303</v>
       </c>
       <c r="D554" s="6" t="s">
         <v>9</v>
@@ -21777,7 +21797,7 @@
     </row>
     <row r="555" spans="1:6" ht="15.75" customHeight="1">
       <c r="B555" s="2" t="s">
-        <v>1301</v>
+        <v>1304</v>
       </c>
       <c r="D555" s="6" t="s">
         <v>3</v>
@@ -21788,7 +21808,7 @@
     </row>
     <row r="556" spans="1:6" ht="15.75" customHeight="1">
       <c r="B556" s="2" t="s">
-        <v>1302</v>
+        <v>1305</v>
       </c>
       <c r="D556" s="6" t="s">
         <v>9</v>
@@ -21799,7 +21819,7 @@
     </row>
     <row r="557" spans="1:6" ht="15.75" customHeight="1">
       <c r="B557" s="2" t="s">
-        <v>1303</v>
+        <v>1306</v>
       </c>
       <c r="D557" s="6" t="s">
         <v>9</v>
@@ -21821,7 +21841,7 @@
     </row>
     <row r="559" spans="1:6" ht="15.75" customHeight="1">
       <c r="B559" s="2" t="s">
-        <v>1304</v>
+        <v>1307</v>
       </c>
       <c r="D559" s="6" t="s">
         <v>9</v>
@@ -21832,7 +21852,7 @@
     </row>
     <row r="560" spans="1:6" ht="15.75" customHeight="1">
       <c r="B560" s="2" t="s">
-        <v>1305</v>
+        <v>1308</v>
       </c>
       <c r="D560" s="6" t="s">
         <v>9</v>
@@ -22216,7 +22236,7 @@
     </row>
     <row r="592" spans="2:8" ht="15.75" customHeight="1">
       <c r="B592" s="2" t="s">
-        <v>1306</v>
+        <v>1309</v>
       </c>
       <c r="D592" s="6" t="s">
         <v>9</v>
@@ -22233,7 +22253,7 @@
         <v>9</v>
       </c>
       <c r="F593" s="2" t="s">
-        <v>1307</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="594" spans="2:6" ht="15.75" customHeight="1">
@@ -22370,24 +22390,24 @@
     </row>
     <row r="606" spans="2:6" ht="15.75" customHeight="1">
       <c r="B606" s="2" t="s">
-        <v>1308</v>
+        <v>1311</v>
       </c>
       <c r="D606" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F606" s="2" t="s">
-        <v>1309</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="607" spans="2:6" ht="15.75" customHeight="1">
       <c r="B607" s="2" t="s">
-        <v>1310</v>
+        <v>1313</v>
       </c>
       <c r="D607" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F607" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
     </row>
   </sheetData>
@@ -22397,8 +22417,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1ef8fdae22ea8efa5f8e6ba78f2f5d7">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a57007e7f6e174e2eadbb94d9d2397b6" ns2:_="" ns3:_="" ns4:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69e77a95-4add-417d-ac50-c09752e64638" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c12e4e740a918a7fed87ba9ba111f97c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e87260b9d5c1107f3f51cd8889399417" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6d852b27-1d95-4577-ac49-0d344a1f93d0"/>
     <xsd:import namespace="fef4af80-67d0-434d-aa7c-17eed15b0840"/>
     <xsd:import namespace="69e77a95-4add-417d-ac50-c09752e64638"/>
@@ -22435,7 +22475,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6d852b27-1d95-4577-ac49-0d344a1f93d0" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="8" nillable="true" ma:displayName="Freigegeben für" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -22454,7 +22494,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="9" nillable="true" ma:displayName="Freigegeben für - Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -22519,7 +22559,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="27f97a9c-5df3-4967-8f8c-2479abf341ed" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildmarkierungen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="27f97a9c-5df3-4967-8f8c-2479abf341ed" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -22566,8 +22606,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Inhaltstyp"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titel"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -22656,28 +22696,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69e77a95-4add-417d-ac50-c09752e64638" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0812515E-9DC9-4E6E-8762-FF0EFB0D58CC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22685,7 +22705,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2C9F8FF-91E5-48A9-94A3-E4B6E752C5B1}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Added new cluster version, new personas&styles, more variation in relation combinations, other minor improvements
</commit_message>
<xml_diff>
--- a/datageneration/data/Spot_primary_keys_bundles.xlsx
+++ b/datageneration/data/Spot_primary_keys_bundles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deutschewelle.sharepoint.com/teams/GR-GR-ReCo-KID2/Freigegebene Dokumente/General/03_Ongoing Work/03C_MS_Spot - ongoing/03Cc_Development/Key-Value Pairs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3166" documentId="8_{B655BF40-E37C-EB41-9787-53099F12E0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A49DA1CD-F918-4C51-8ED2-43B67EDC81E4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4DBD36D-58F0-474F-BD74-65009DB0B6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14420" yWindow="500" windowWidth="35300" windowHeight="26260" xr2:uid="{0ED01DE8-A235-1045-8C96-52557544134F}"/>
   </bookViews>
@@ -2777,7 +2777,7 @@
     <t>landuse=logging, man_made=clearcut, man_made=cutline</t>
   </si>
   <si>
-    <t>street lane|Car lane|traffic lane|lanes|with more than X lanes|which has X lanes</t>
+    <t>street lanes|number of car lanes|traffic lanes|number of lanes|with more than X lanes|which has X lanes</t>
   </si>
   <si>
     <t>lanes=***numeric***</t>
@@ -3527,7 +3527,7 @@
     <t>emergency=water_rescue</t>
   </si>
   <si>
-    <t>wi-fi hotspot|wi-fi|public wifi|hotspot</t>
+    <t>wi-fi hotspot|wi-fi|public wifi</t>
   </si>
   <si>
     <t>internet_access=wlan</t>
@@ -4679,8 +4679,8 @@
   <dimension ref="A1:I613"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+      <pane ySplit="1" topLeftCell="A532" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C556" sqref="C556"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" customHeight="1"/>
@@ -11546,11 +11546,11 @@
         <v>882</v>
       </c>
     </row>
-    <row r="433" spans="1:7">
+    <row r="433" spans="1:7" ht="32.25">
       <c r="A433" s="2">
         <v>9007</v>
       </c>
-      <c r="B433" s="2" t="s">
+      <c r="B433" s="5" t="s">
         <v>883</v>
       </c>
       <c r="D433" s="6" t="s">
@@ -13163,7 +13163,7 @@
         <v>1133</v>
       </c>
       <c r="D558" s="6" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="G558" s="2" t="s">
         <v>1134</v>
@@ -22776,26 +22776,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="69e77a95-4add-417d-ac50-c09752e64638" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100BB17A56B5CDE7946ADE40FE50F9E0E05" ma:contentTypeVersion="18" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c12e4e740a918a7fed87ba9ba111f97c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6d852b27-1d95-4577-ac49-0d344a1f93d0" xmlns:ns3="fef4af80-67d0-434d-aa7c-17eed15b0840" xmlns:ns4="69e77a95-4add-417d-ac50-c09752e64638" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e87260b9d5c1107f3f51cd8889399417" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="6d852b27-1d95-4577-ac49-0d344a1f93d0"/>
@@ -23055,16 +23035,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="fef4af80-67d0-434d-aa7c-17eed15b0840">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="69e77a95-4add-417d-ac50-c09752e64638" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2C9F8FF-91E5-48A9-94A3-E4B6E752C5B1}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E49D155-2C11-4885-ACD3-E6D3BF89105E}"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2787CFFA-3460-4A04-BA0A-9FECDEAA6229}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2C9F8FF-91E5-48A9-94A3-E4B6E752C5B1}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>